<commit_message>
New consists fragments Plan W
</commit_message>
<xml_diff>
--- a/RailWorks/Source/RailionLudmilla-Consists/Materieel/Rijtuigen/overzicht-inzet.xlsx
+++ b/RailWorks/Source/RailionLudmilla-Consists/Materieel/Rijtuigen/overzicht-inzet.xlsx
@@ -8,12 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Games\Steam\steamapps\common\RailWorks\Source\RailionLudmilla-Consists\Materieel\Rijtuigen\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1CB179F8-AD5A-47D2-A63B-D95BDD265612}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{256F472D-DA0D-4368-BFD9-C7583775FF5E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="14400" windowHeight="15600" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="14400" yWindow="0" windowWidth="14400" windowHeight="15600" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="ICR" sheetId="1" r:id="rId1"/>
+    <sheet name="Plan W" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -182,8 +183,212 @@
 </comments>
 </file>
 
+<file path=xl/comments2.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
+  <authors>
+    <author>Tom</author>
+  </authors>
+  <commentList>
+    <comment ref="A1" authorId="0" shapeId="0" xr:uid="{CEE0F991-71E5-4E1F-A35A-85DBA5145ADA}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Tom:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+W1: nummer eindigt op 4xx
+W2: nummer eindigt op 5xx</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="A2" authorId="0" shapeId="0" xr:uid="{5B3E9958-933D-4EE5-A4B3-39384BEC44DE}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Tom:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+slechts 3 rijtuigen, rest was Bnl</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="A3" authorId="0" shapeId="0" xr:uid="{085F7D9D-C4DD-425B-A842-64C7444DE888}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Tom:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+'73 op railwiki</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="A4" authorId="0" shapeId="0" xr:uid="{A7122EB4-7A95-4183-AD1A-07E1EE6C9FAC}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Tom:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+andere ramen</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="C6" authorId="0" shapeId="0" xr:uid="{5398D912-08D9-42BF-86E7-7BAE2EA846B2}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Tom:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+herindienststelling</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="A8" authorId="0" shapeId="0" xr:uid="{DFF8A1D1-7519-4195-B8F9-E5EC95FCCEA3}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Tom:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+blauw met gele deuren
+enkel rijtuig: 507</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="A9" authorId="0" shapeId="0" xr:uid="{4D199028-542A-4062-A684-51D377355B62}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Tom:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+herkenbaar aan nummer rechts ipv midden</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="C10" authorId="0" shapeId="0" xr:uid="{4EBA6DD3-4035-4F4E-8B87-BF9290307E8A}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Tom:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+herindienststelling</t>
+        </r>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="34">
   <si>
     <t>ICR benelux</t>
   </si>
@@ -258,6 +463,33 @@
   </si>
   <si>
     <t>Zie ook v250.nl</t>
+  </si>
+  <si>
+    <t>84?</t>
+  </si>
+  <si>
+    <t>82?</t>
+  </si>
+  <si>
+    <t>Plan W1 blauw '74</t>
+  </si>
+  <si>
+    <t>Plan W1 benelux '74</t>
+  </si>
+  <si>
+    <t>Plan W1 benelux '84</t>
+  </si>
+  <si>
+    <t>Plan W1 ic '87</t>
+  </si>
+  <si>
+    <t>Plan W2 ic '82</t>
+  </si>
+  <si>
+    <t>Plan W2 blauw rb '68</t>
+  </si>
+  <si>
+    <t>Plan W2 507 '81</t>
   </si>
 </sst>
 </file>
@@ -265,9 +497,9 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
-    <numFmt numFmtId="166" formatCode="[$-413]mmm/yy;@"/>
+    <numFmt numFmtId="164" formatCode="[$-413]mmm/yy;@"/>
   </numFmts>
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -296,6 +528,19 @@
       <name val="Tahoma"/>
       <family val="2"/>
     </font>
+    <font>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="Tahoma"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="Tahoma"/>
+      <charset val="1"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -321,8 +566,8 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="17" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="166" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Standaard" xfId="0" builtinId="0"/>
@@ -605,8 +850,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:D39"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="A39" sqref="A39"/>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:D1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -943,4 +1188,135 @@
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>
   <legacyDrawing r:id="rId2"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{34F6A220-FD91-4F5A-ACFA-A0D4B83AD909}">
+  <dimension ref="A1:D10"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D19" sqref="D19"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <cols>
+    <col min="1" max="1" width="3" customWidth="1"/>
+    <col min="2" max="2" width="16.33203125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A1" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B1" s="3"/>
+      <c r="C1" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="D1" s="3" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A2" t="s">
+        <v>27</v>
+      </c>
+      <c r="C2" s="2">
+        <v>25750</v>
+      </c>
+      <c r="D2" s="2">
+        <v>32417</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A3" t="s">
+        <v>28</v>
+      </c>
+      <c r="C3" s="2">
+        <v>26816</v>
+      </c>
+      <c r="D3" s="2" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A4" t="s">
+        <v>29</v>
+      </c>
+      <c r="C4" t="s">
+        <v>26</v>
+      </c>
+      <c r="D4" s="2">
+        <v>32417</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A5" t="s">
+        <v>30</v>
+      </c>
+      <c r="C5" s="2">
+        <v>31929</v>
+      </c>
+      <c r="D5" s="2">
+        <v>35217</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A6" t="s">
+        <v>30</v>
+      </c>
+      <c r="C6" s="2">
+        <v>35916</v>
+      </c>
+      <c r="D6" s="2">
+        <v>37956</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A7" t="s">
+        <v>32</v>
+      </c>
+      <c r="C7" s="2">
+        <v>25020</v>
+      </c>
+      <c r="D7" s="2">
+        <v>30682</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A8" t="s">
+        <v>33</v>
+      </c>
+      <c r="C8" s="2">
+        <v>29891</v>
+      </c>
+      <c r="D8" s="2">
+        <v>30256</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A9" t="s">
+        <v>31</v>
+      </c>
+      <c r="C9" s="2">
+        <v>30256</v>
+      </c>
+      <c r="D9" s="2">
+        <v>35309</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A10" t="s">
+        <v>31</v>
+      </c>
+      <c r="C10" s="2">
+        <v>35916</v>
+      </c>
+      <c r="D10" s="2">
+        <v>37956</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <legacyDrawing r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
DDM1 fragments volgens railwiki
</commit_message>
<xml_diff>
--- a/RailWorks/Source/RailionLudmilla-Consists/Materieel/Rijtuigen/overzicht-inzet.xlsx
+++ b/RailWorks/Source/RailionLudmilla-Consists/Materieel/Rijtuigen/overzicht-inzet.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Games\Steam\steamapps\common\RailWorks\Source\RailionLudmilla-Consists\Materieel\Rijtuigen\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{203FD923-46FD-46A2-AD42-49C8C1DB61A0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CAE6C7E7-F8D4-42D0-A15C-12C05F10A85C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="14400" windowHeight="15600" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -658,12 +658,36 @@
         </r>
       </text>
     </comment>
+    <comment ref="B40" authorId="0" shapeId="0" xr:uid="{F0DF2EAD-27DB-4EFB-8795-8D91D4666612}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Tom:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+kan geen data vinden over eerdere stammen</t>
+        </r>
+      </text>
+    </comment>
   </commentList>
 </comments>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="95" uniqueCount="55">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="104" uniqueCount="62">
   <si>
     <t>ICR benelux</t>
   </si>
@@ -828,6 +852,27 @@
   </si>
   <si>
     <t>Consists</t>
+  </si>
+  <si>
+    <t>DDM1 7 1985</t>
+  </si>
+  <si>
+    <t>DDM1 6 1985</t>
+  </si>
+  <si>
+    <t>DDM1 7 1993</t>
+  </si>
+  <si>
+    <t>DDM1 5 1995</t>
+  </si>
+  <si>
+    <t>DDM1 7 1999</t>
+  </si>
+  <si>
+    <t>DDM1 6 2004</t>
+  </si>
+  <si>
+    <t>DDM1 4 2016</t>
   </si>
 </sst>
 </file>
@@ -1661,10 +1706,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C42AD58B-783D-4A65-88F6-4F4D48B1C5CA}">
-  <dimension ref="A1:K36"/>
+  <dimension ref="A1:K43"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="A36" sqref="A36"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E37" sqref="E37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -1928,9 +1973,92 @@
         <v>49</v>
       </c>
     </row>
-    <row r="36" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="36" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A36" s="1" t="s">
         <v>54</v>
+      </c>
+      <c r="B36" t="s">
+        <v>7</v>
+      </c>
+      <c r="C36" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="37" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A37" t="s">
+        <v>61</v>
+      </c>
+      <c r="B37" s="2">
+        <v>42522</v>
+      </c>
+      <c r="C37" s="2">
+        <v>43800</v>
+      </c>
+    </row>
+    <row r="38" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A38" t="s">
+        <v>58</v>
+      </c>
+      <c r="B38" s="2">
+        <v>34851</v>
+      </c>
+      <c r="C38" s="2">
+        <v>37591</v>
+      </c>
+    </row>
+    <row r="39" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A39" t="s">
+        <v>56</v>
+      </c>
+      <c r="B39" s="2">
+        <v>31199</v>
+      </c>
+      <c r="C39" s="2">
+        <v>34851</v>
+      </c>
+    </row>
+    <row r="40" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A40" t="s">
+        <v>60</v>
+      </c>
+      <c r="B40" s="2">
+        <v>37043</v>
+      </c>
+      <c r="C40" s="2">
+        <v>41244</v>
+      </c>
+    </row>
+    <row r="41" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A41" t="s">
+        <v>55</v>
+      </c>
+      <c r="B41" s="2">
+        <v>31199</v>
+      </c>
+      <c r="C41" s="2">
+        <v>34121</v>
+      </c>
+    </row>
+    <row r="42" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A42" t="s">
+        <v>57</v>
+      </c>
+      <c r="B42" s="2">
+        <v>34121</v>
+      </c>
+      <c r="C42" s="2">
+        <v>36312</v>
+      </c>
+    </row>
+    <row r="43" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A43" t="s">
+        <v>59</v>
+      </c>
+      <c r="B43" s="2">
+        <v>36312</v>
+      </c>
+      <c r="C43" s="2">
+        <v>37956</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
DDM1 samenstellingen compleet, nog niet geflipt
</commit_message>
<xml_diff>
--- a/RailWorks/Source/RailionLudmilla-Consists/Materieel/Rijtuigen/overzicht-inzet.xlsx
+++ b/RailWorks/Source/RailionLudmilla-Consists/Materieel/Rijtuigen/overzicht-inzet.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Games\Steam\steamapps\common\RailWorks\Source\RailionLudmilla-Consists\Materieel\Rijtuigen\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3E07D787-6EF5-4E28-9BB6-7B868FFC004B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{03D8FA33-4E5D-49DD-A5A6-5E372D79D450}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="14400" windowHeight="15600" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -394,151 +394,7 @@
     <author>Tom</author>
   </authors>
   <commentList>
-    <comment ref="A9" authorId="0" shapeId="0" xr:uid="{AA0101F6-AD08-422A-A55B-C2CD727AC770}">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <charset val="1"/>
-          </rPr>
-          <t>Tom:</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <charset val="1"/>
-          </rPr>
-          <t xml:space="preserve">
-Let op later soms ook icm 1700!</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="A12" authorId="0" shapeId="0" xr:uid="{8138D36A-AF0C-47BD-9E7A-49120B836CD6}">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <charset val="1"/>
-          </rPr>
-          <t>Tom:</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <charset val="1"/>
-          </rPr>
-          <t xml:space="preserve">
-indeling wordt tussendoor gewijzigd volgens railwiki?</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="B13" authorId="0" shapeId="0" xr:uid="{1EEDF551-8EB3-4617-8E8D-2C30F2359817}">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <charset val="1"/>
-          </rPr>
-          <t>Tom:</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <charset val="1"/>
-          </rPr>
-          <t xml:space="preserve">
-volgens railwiki vanaf 2004</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="C13" authorId="0" shapeId="0" xr:uid="{59DD633A-A456-438B-858E-17EF210C6DB5}">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <charset val="1"/>
-          </rPr>
-          <t>Tom:</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <charset val="1"/>
-          </rPr>
-          <t xml:space="preserve">
-klopt met railwiki</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="A15" authorId="0" shapeId="0" xr:uid="{E675E8B2-D0B9-42E0-B2E4-F260D30F84E3}">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <charset val="1"/>
-          </rPr>
-          <t>Tom:</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <charset val="1"/>
-          </rPr>
-          <t xml:space="preserve">
-niet bevestigd door railwiki</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="B16" authorId="0" shapeId="0" xr:uid="{A1A0A7E1-F8A9-4C39-B351-C27E085590B7}">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <charset val="1"/>
-          </rPr>
-          <t>Tom:</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <charset val="1"/>
-          </rPr>
-          <t xml:space="preserve">
-klopt met railwiki</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="E23" authorId="0" shapeId="0" xr:uid="{7A3C02EA-EF21-4F8D-8D86-BAF1B29EA7C7}">
+    <comment ref="E8" authorId="0" shapeId="0" xr:uid="{7A3C02EA-EF21-4F8D-8D86-BAF1B29EA7C7}">
       <text>
         <r>
           <rPr>
@@ -562,7 +418,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="C24" authorId="0" shapeId="0" xr:uid="{7884F449-2FCC-449A-A56E-A6834E5F3276}">
+    <comment ref="C9" authorId="0" shapeId="0" xr:uid="{7884F449-2FCC-449A-A56E-A6834E5F3276}">
       <text>
         <r>
           <rPr>
@@ -586,7 +442,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="H24" authorId="0" shapeId="0" xr:uid="{6C8EA8AF-4C6F-4FE0-9F8B-14B78D398EFE}">
+    <comment ref="H9" authorId="0" shapeId="0" xr:uid="{6C8EA8AF-4C6F-4FE0-9F8B-14B78D398EFE}">
       <text>
         <r>
           <rPr>
@@ -610,7 +466,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="C25" authorId="0" shapeId="0" xr:uid="{F10A9C2C-3651-4ADC-A417-6C94B13D50BE}">
+    <comment ref="C10" authorId="0" shapeId="0" xr:uid="{F10A9C2C-3651-4ADC-A417-6C94B13D50BE}">
       <text>
         <r>
           <rPr>
@@ -634,7 +490,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="E25" authorId="0" shapeId="0" xr:uid="{0AAF0B79-7C4E-4305-9801-242211730F3E}">
+    <comment ref="E10" authorId="0" shapeId="0" xr:uid="{0AAF0B79-7C4E-4305-9801-242211730F3E}">
       <text>
         <r>
           <rPr>
@@ -658,7 +514,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="B40" authorId="0" shapeId="0" xr:uid="{F0DF2EAD-27DB-4EFB-8795-8D91D4666612}">
+    <comment ref="B25" authorId="0" shapeId="0" xr:uid="{F0DF2EAD-27DB-4EFB-8795-8D91D4666612}">
       <text>
         <r>
           <rPr>
@@ -687,7 +543,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="108" uniqueCount="66">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="95" uniqueCount="59">
   <si>
     <t>ICR benelux</t>
   </si>
@@ -800,24 +656,6 @@
     <t>Rijtuigen zijn in het echt willekeurig geflipt. Zoek wat foto's op nadat de samenstellingen compleet zijn</t>
   </si>
   <si>
-    <t>DDM1 4</t>
-  </si>
-  <si>
-    <t>DDM1 5</t>
-  </si>
-  <si>
-    <t>DDM1 6</t>
-  </si>
-  <si>
-    <t>DDM1 6 alt</t>
-  </si>
-  <si>
-    <t>DDM1 7</t>
-  </si>
-  <si>
-    <t>Op basis van Flickr:</t>
-  </si>
-  <si>
     <t>Lengtes volgens railwiki</t>
   </si>
   <si>
@@ -846,9 +684,6 @@
   </si>
   <si>
     <t>in dienst</t>
-  </si>
-  <si>
-    <t>TODO: loop samenstellingen na obv "lengtes volgens railwiki" hieronder</t>
   </si>
   <si>
     <t>Consists</t>
@@ -1718,10 +1553,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C42AD58B-783D-4A65-88F6-4F4D48B1C5CA}">
-  <dimension ref="A1:K47"/>
+  <dimension ref="A1:K32"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F12" sqref="F12"/>
+      <selection activeCell="E11" sqref="E11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -1729,371 +1564,273 @@
     <col min="1" max="1" width="18.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A1" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A2" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A3" s="1" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.45">
-      <c r="A5" s="1" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.45">
-      <c r="A7" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.45">
-      <c r="B9" t="s">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.45">
+      <c r="A5" s="1"/>
+    </row>
+    <row r="6" spans="1:11" x14ac:dyDescent="0.45">
+      <c r="A6" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="B6" s="2">
+        <v>31199</v>
+      </c>
+      <c r="C6" s="2">
+        <v>34121</v>
+      </c>
+      <c r="D6" s="2">
+        <v>34851</v>
+      </c>
+      <c r="E6" s="2">
+        <v>36312</v>
+      </c>
+      <c r="F6" s="2">
+        <v>37043</v>
+      </c>
+      <c r="G6" s="2">
+        <v>37622</v>
+      </c>
+      <c r="H6" s="2">
+        <v>37987</v>
+      </c>
+      <c r="I6" s="2">
+        <v>41244</v>
+      </c>
+      <c r="J6" s="2">
+        <v>42522</v>
+      </c>
+      <c r="K6" s="2">
+        <v>43800</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11" x14ac:dyDescent="0.45">
+      <c r="A7">
+        <v>4</v>
+      </c>
+      <c r="B7" s="2"/>
+      <c r="C7" s="2"/>
+      <c r="J7" t="s">
+        <v>46</v>
+      </c>
+      <c r="K7" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11" x14ac:dyDescent="0.45">
+      <c r="A8">
+        <v>5</v>
+      </c>
+      <c r="B8" s="2"/>
+      <c r="C8" s="2"/>
+      <c r="D8" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="E8" t="s">
+        <v>44</v>
+      </c>
+      <c r="F8" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11" x14ac:dyDescent="0.45">
+      <c r="A9">
+        <v>6</v>
+      </c>
+      <c r="B9" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="C9" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="F9" t="s">
+        <v>44</v>
+      </c>
+      <c r="G9" t="s">
+        <v>44</v>
+      </c>
+      <c r="H9" t="s">
+        <v>44</v>
+      </c>
+      <c r="I9" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="10" spans="1:11" x14ac:dyDescent="0.45">
+      <c r="A10">
         <v>7</v>
       </c>
-      <c r="C9" t="s">
-        <v>8</v>
-      </c>
-      <c r="D9" t="s">
-        <v>7</v>
-      </c>
-      <c r="E9" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.45">
-      <c r="A10" t="s">
-        <v>41</v>
-      </c>
-      <c r="B10" s="2">
-        <v>31260</v>
-      </c>
-      <c r="C10" s="2">
-        <v>31260</v>
-      </c>
-    </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.45">
-      <c r="A11" t="s">
-        <v>40</v>
-      </c>
-      <c r="B11" s="2">
-        <v>33270</v>
-      </c>
-      <c r="C11" s="2">
-        <v>33270</v>
-      </c>
-    </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="B10" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="C10" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="D10" t="s">
+        <v>44</v>
+      </c>
+      <c r="E10" t="s">
+        <v>44</v>
+      </c>
+      <c r="F10" t="s">
+        <v>44</v>
+      </c>
+      <c r="G10" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="12" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A12" t="s">
         <v>38</v>
       </c>
-      <c r="B12" s="2">
+    </row>
+    <row r="13" spans="1:11" x14ac:dyDescent="0.45">
+      <c r="A13" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="14" spans="1:11" x14ac:dyDescent="0.45">
+      <c r="A14" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="15" spans="1:11" x14ac:dyDescent="0.45">
+      <c r="A15" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="16" spans="1:11" x14ac:dyDescent="0.45">
+      <c r="A16" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A17" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A21" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="B21" t="s">
+        <v>7</v>
+      </c>
+      <c r="C21" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A22" t="s">
+        <v>54</v>
+      </c>
+      <c r="B22" s="2">
+        <v>42522</v>
+      </c>
+      <c r="C22" s="2">
+        <v>43800</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A23" t="s">
+        <v>51</v>
+      </c>
+      <c r="B23" s="2">
         <v>34851</v>
       </c>
-      <c r="C12" s="2">
+      <c r="C23" s="2">
         <v>37591</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.45">
-      <c r="A13" t="s">
-        <v>39</v>
-      </c>
-      <c r="B13" s="2">
-        <v>38718</v>
-      </c>
-      <c r="C13" s="2">
-        <v>41395</v>
-      </c>
-    </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.45">
-      <c r="A14" t="s">
-        <v>40</v>
-      </c>
-      <c r="D14" s="2">
-        <v>40940</v>
-      </c>
-      <c r="E14" s="2">
-        <v>40940</v>
-      </c>
-    </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.45">
-      <c r="A15" t="s">
-        <v>38</v>
-      </c>
-      <c r="B15" s="2">
-        <v>39630</v>
-      </c>
-      <c r="C15" s="2">
-        <v>39630</v>
-      </c>
-    </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.45">
-      <c r="A16" t="s">
-        <v>37</v>
-      </c>
-      <c r="B16" s="2">
-        <v>42430</v>
-      </c>
-      <c r="C16" s="2">
-        <v>43800</v>
-      </c>
-    </row>
-    <row r="21" spans="1:11" x14ac:dyDescent="0.45">
-      <c r="A21" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="B21" s="2">
+    <row r="24" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A24" t="s">
+        <v>49</v>
+      </c>
+      <c r="B24" s="2">
         <v>31199</v>
       </c>
-      <c r="C21" s="2">
+      <c r="C24" s="2">
+        <v>34851</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A25" t="s">
+        <v>53</v>
+      </c>
+      <c r="B25" s="2">
+        <v>37043</v>
+      </c>
+      <c r="C25" s="2">
+        <v>41244</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A26" t="s">
+        <v>48</v>
+      </c>
+      <c r="B26" s="2">
+        <v>31199</v>
+      </c>
+      <c r="C26" s="2">
         <v>34121</v>
       </c>
-      <c r="D21" s="2">
-        <v>34851</v>
-      </c>
-      <c r="E21" s="2">
+    </row>
+    <row r="27" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A27" t="s">
+        <v>50</v>
+      </c>
+      <c r="B27" s="2">
+        <v>34121</v>
+      </c>
+      <c r="C27" s="2">
         <v>36312</v>
       </c>
-      <c r="F21" s="2">
-        <v>37043</v>
-      </c>
-      <c r="G21" s="2">
-        <v>37622</v>
-      </c>
-      <c r="H21" s="2">
-        <v>37987</v>
-      </c>
-      <c r="I21" s="2">
-        <v>41244</v>
-      </c>
-      <c r="J21" s="2">
-        <v>42522</v>
-      </c>
-      <c r="K21" s="2">
-        <v>43800</v>
-      </c>
-    </row>
-    <row r="22" spans="1:11" x14ac:dyDescent="0.45">
-      <c r="A22">
-        <v>4</v>
-      </c>
-      <c r="B22" s="2"/>
-      <c r="C22" s="2"/>
-      <c r="J22" t="s">
+    </row>
+    <row r="28" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A28" t="s">
         <v>52</v>
       </c>
-      <c r="K22" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="23" spans="1:11" x14ac:dyDescent="0.45">
-      <c r="A23">
-        <v>5</v>
-      </c>
-      <c r="B23" s="2"/>
-      <c r="C23" s="2"/>
-      <c r="D23" s="2" t="s">
-        <v>50</v>
-      </c>
-      <c r="E23" t="s">
-        <v>50</v>
-      </c>
-      <c r="F23" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="24" spans="1:11" x14ac:dyDescent="0.45">
-      <c r="A24">
-        <v>6</v>
-      </c>
-      <c r="B24" s="2" t="s">
-        <v>50</v>
-      </c>
-      <c r="C24" s="2" t="s">
-        <v>50</v>
-      </c>
-      <c r="F24" t="s">
-        <v>50</v>
-      </c>
-      <c r="G24" t="s">
-        <v>50</v>
-      </c>
-      <c r="H24" t="s">
-        <v>50</v>
-      </c>
-      <c r="I24" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="25" spans="1:11" x14ac:dyDescent="0.45">
-      <c r="A25">
-        <v>7</v>
-      </c>
-      <c r="B25" s="2" t="s">
-        <v>50</v>
-      </c>
-      <c r="C25" s="2" t="s">
-        <v>50</v>
-      </c>
-      <c r="D25" t="s">
-        <v>50</v>
-      </c>
-      <c r="E25" t="s">
-        <v>50</v>
-      </c>
-      <c r="F25" t="s">
-        <v>50</v>
-      </c>
-      <c r="G25" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="27" spans="1:11" x14ac:dyDescent="0.45">
-      <c r="A27" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="28" spans="1:11" x14ac:dyDescent="0.45">
-      <c r="A28" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="29" spans="1:11" x14ac:dyDescent="0.45">
-      <c r="A29" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="30" spans="1:11" x14ac:dyDescent="0.45">
+      <c r="B28" s="2">
+        <v>36312</v>
+      </c>
+      <c r="C28" s="2">
+        <v>37956</v>
+      </c>
+    </row>
+    <row r="30" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A30" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="31" spans="1:11" x14ac:dyDescent="0.45">
+        <v>57</v>
+      </c>
+      <c r="B30" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="31" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A31" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="32" spans="1:11" x14ac:dyDescent="0.45">
-      <c r="A32" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="36" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="A36" s="1" t="s">
-        <v>54</v>
-      </c>
-      <c r="B36" t="s">
-        <v>7</v>
-      </c>
-      <c r="C36" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="37" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="A37" t="s">
-        <v>61</v>
-      </c>
-      <c r="B37" s="2">
-        <v>42522</v>
-      </c>
-      <c r="C37" s="2">
-        <v>43800</v>
-      </c>
-    </row>
-    <row r="38" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="A38" t="s">
-        <v>58</v>
-      </c>
-      <c r="B38" s="2">
-        <v>34851</v>
-      </c>
-      <c r="C38" s="2">
-        <v>37591</v>
-      </c>
-    </row>
-    <row r="39" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="A39" t="s">
+        <v>55</v>
+      </c>
+      <c r="B31" s="2">
+        <v>40817</v>
+      </c>
+      <c r="C31" s="2" t="s">
         <v>56</v>
       </c>
-      <c r="B39" s="2">
-        <v>31199</v>
-      </c>
-      <c r="C39" s="2">
-        <v>34851</v>
-      </c>
-    </row>
-    <row r="40" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="A40" t="s">
-        <v>60</v>
-      </c>
-      <c r="B40" s="2">
-        <v>37043</v>
-      </c>
-      <c r="C40" s="2">
-        <v>41244</v>
-      </c>
-    </row>
-    <row r="41" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="A41" t="s">
-        <v>55</v>
-      </c>
-      <c r="B41" s="2">
-        <v>31199</v>
-      </c>
-      <c r="C41" s="2">
-        <v>34121</v>
-      </c>
-    </row>
-    <row r="42" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="A42" t="s">
-        <v>57</v>
-      </c>
-      <c r="B42" s="2">
-        <v>34121</v>
-      </c>
-      <c r="C42" s="2">
-        <v>36312</v>
-      </c>
-    </row>
-    <row r="43" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="A43" t="s">
-        <v>59</v>
-      </c>
-      <c r="B43" s="2">
-        <v>36312</v>
-      </c>
-      <c r="C43" s="2">
-        <v>37956</v>
-      </c>
-    </row>
-    <row r="45" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="A45" t="s">
-        <v>64</v>
-      </c>
-      <c r="B45" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="46" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="A46" t="s">
-        <v>62</v>
-      </c>
-      <c r="B46" s="2">
-        <v>40817</v>
-      </c>
-      <c r="C46" s="2" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="47" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="B47" s="2"/>
+    </row>
+    <row r="32" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="B32" s="2"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Finish DDM-1 new consists
</commit_message>
<xml_diff>
--- a/RailWorks/Source/RailionLudmilla-Consists/Materieel/Rijtuigen/overzicht-inzet.xlsx
+++ b/RailWorks/Source/RailionLudmilla-Consists/Materieel/Rijtuigen/overzicht-inzet.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Games\Steam\steamapps\common\RailWorks\Source\RailionLudmilla-Consists\Materieel\Rijtuigen\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E3A330B8-76A7-4D70-B9AB-D7B6D6736C5E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F603DEA3-3AB9-4D12-9C0D-FE5673C50441}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="14400" windowHeight="15600" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="14400" yWindow="0" windowWidth="14400" windowHeight="15600" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="ICR" sheetId="1" r:id="rId1"/>
@@ -706,6 +706,30 @@
         </r>
       </text>
     </comment>
+    <comment ref="B30" authorId="0" shapeId="0" xr:uid="{0A7EA9CB-9940-42F0-BCFE-2561BE76967A}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Tom:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+voor eenvoud laten starten vanaf jun-99</t>
+        </r>
+      </text>
+    </comment>
   </commentList>
 </comments>
 </file>
@@ -887,7 +911,7 @@
     <t>1800 ipv 1600</t>
   </si>
   <si>
-    <t>zie 1800 consists, rond 1999</t>
+    <t>begin 99</t>
   </si>
 </sst>
 </file>
@@ -1885,12 +1909,12 @@
         <v>40</v>
       </c>
     </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A17" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="21" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A21" s="1" t="s">
         <v>47</v>
       </c>
@@ -1901,7 +1925,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="22" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A22" t="s">
         <v>54</v>
       </c>
@@ -1912,7 +1936,7 @@
         <v>43800</v>
       </c>
     </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="23" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A23" t="s">
         <v>51</v>
       </c>
@@ -1923,7 +1947,7 @@
         <v>37591</v>
       </c>
     </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="24" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A24" t="s">
         <v>49</v>
       </c>
@@ -1934,7 +1958,7 @@
         <v>34851</v>
       </c>
     </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="25" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A25" t="s">
         <v>53</v>
       </c>
@@ -1945,7 +1969,7 @@
         <v>41244</v>
       </c>
     </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="26" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A26" t="s">
         <v>48</v>
       </c>
@@ -1956,7 +1980,7 @@
         <v>34121</v>
       </c>
     </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="27" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A27" t="s">
         <v>50</v>
       </c>
@@ -1967,7 +1991,7 @@
         <v>36312</v>
       </c>
     </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="28" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A28" t="s">
         <v>52</v>
       </c>
@@ -1978,15 +2002,16 @@
         <v>37956</v>
       </c>
     </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="30" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A30" t="s">
         <v>57</v>
       </c>
       <c r="B30" t="s">
         <v>58</v>
       </c>
-    </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="E30" s="2"/>
+    </row>
+    <row r="31" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A31" t="s">
         <v>55</v>
       </c>
@@ -1997,7 +2022,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="32" spans="1:5" x14ac:dyDescent="0.45">
       <c r="B32" s="2"/>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
WIP ICR and research
</commit_message>
<xml_diff>
--- a/RailWorks/Source/RailionLudmilla-Consists/Materieel/Rijtuigen/overzicht-inzet.xlsx
+++ b/RailWorks/Source/RailionLudmilla-Consists/Materieel/Rijtuigen/overzicht-inzet.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Games\Steam\steamapps\common\RailWorks\Source\RailionLudmilla-Consists\Materieel\Rijtuigen\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F603DEA3-3AB9-4D12-9C0D-FE5673C50441}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E385E382-57E2-424B-9445-86525F99945D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="14400" yWindow="0" windowWidth="14400" windowHeight="15600" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="14400" windowHeight="15600" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="ICR" sheetId="1" r:id="rId1"/>
@@ -180,6 +180,272 @@
         </r>
       </text>
     </comment>
+    <comment ref="A77" authorId="0" shapeId="0" xr:uid="{A8C4BB1C-E598-4BBC-8FDD-3D666EB65BF9}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Tom:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+TODO 1980-1985 ivm Plan E
+TODO video nodig voor langere samenstellingen
+TODO na 2015 ivm ICRmh</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="B80" authorId="0" shapeId="0" xr:uid="{468F2A97-B0ED-43C2-AC20-CE363788D779}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Tom:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+1x Benelux</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="B82" authorId="0" shapeId="0" xr:uid="{ECEB2C0C-B792-4B89-AAC3-C86274139980}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Tom:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+1x Benelux B</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="B83" authorId="0" shapeId="0" xr:uid="{2B83792C-45C9-4B9E-AD67-C24AED65ACD9}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Tom:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+1x Benelux BKD</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="B97" authorId="0" shapeId="0" xr:uid="{0EA34362-894E-4678-8674-8E5A71C685EB}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Tom:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+Fyra, NS, Benelux, Benelux Bs</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="B98" authorId="0" shapeId="0" xr:uid="{154791C1-5BB9-4708-B36B-EBB1EF1E5330}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Tom:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+Fyra, Fyra Bs</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="B99" authorId="0" shapeId="0" xr:uid="{7807BECB-78A6-4F35-8B16-EE147C59E778}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Tom:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+Fyra, Benelux Bs</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="B100" authorId="0" shapeId="0" xr:uid="{05376CFB-963C-47DE-855B-52E21973DF19}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Tom:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+Fyra, NS, Benelux Bs</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="B101" authorId="0" shapeId="0" xr:uid="{FBA2AC70-588E-440C-8101-8A4DBE3A14B7}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Tom:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+Fyra, Benelux Bs</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="B104" authorId="0" shapeId="0" xr:uid="{DFA5F928-8F7A-4EE7-B4D0-0A95A03301C5}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Tom:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+Fyra met logo, NS, Benelux Bs</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="B106" authorId="0" shapeId="0" xr:uid="{EF7BC567-5EC7-4577-89BF-EBCD72B89596}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Tom:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+Nog compleet Fyra</t>
+        </r>
+      </text>
+    </comment>
   </commentList>
 </comments>
 </file>
@@ -735,7 +1001,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="95" uniqueCount="59">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="165" uniqueCount="125">
   <si>
     <t>ICR benelux</t>
   </si>
@@ -912,6 +1178,204 @@
   </si>
   <si>
     <t>begin 99</t>
+  </si>
+  <si>
+    <t>1980: vaak A+BKD+B+B plus versterking</t>
+  </si>
+  <si>
+    <t>1988: Duitse rijtuigen in trein naar Keulen, ICR als versterking</t>
+  </si>
+  <si>
+    <t>1991 (jan): Twee 12-rijtuig composities in 800/900</t>
+  </si>
+  <si>
+    <t>1986 (okt): eerste benelux, HLE11+BKD+A+AB+B+B+Bs</t>
+  </si>
+  <si>
+    <t>1994 (jun): trein naar Keulen is weer ICR. Gemiddeld A+BKD+B+B plus 3 versterkingsrijtuigen</t>
+  </si>
+  <si>
+    <t>1998 (voorjaar): inkorting benelux tot 6 rijtuigen</t>
+  </si>
+  <si>
+    <t>Samenstellingen (railwiki)</t>
+  </si>
+  <si>
+    <t>1999 (aug): ijsellijn: 1700+6xICR+1700</t>
+  </si>
+  <si>
+    <t>1999 (sep): DDM-1 Bv vervangt B in ijsellijn stam</t>
+  </si>
+  <si>
+    <t>2002 (feb): DD-AR Bvk combinaties: Bvk+B+A+BKD+B</t>
+  </si>
+  <si>
+    <t>2003: instroom ICK</t>
+  </si>
+  <si>
+    <t>2003: na ICRm revisie combinaties met vanalles: ICR, Plan W, DDM-1, ICK, K4</t>
+  </si>
+  <si>
+    <t>2004: instroom BDs. Regelmatig vervangen door loc ivm storing</t>
+  </si>
+  <si>
+    <t>2007: composities van 11 en 7 rijtuigen</t>
+  </si>
+  <si>
+    <t>2011: 7-delige en 10-delige stammen</t>
+  </si>
+  <si>
+    <t>2013 (sep): inkorting 10-delige stammen naar 9-delig. Vaste composities 7-delig (15700) en 9-delig (15100)</t>
+  </si>
+  <si>
+    <t>2014: 7-delig, 9-delig</t>
+  </si>
+  <si>
+    <t>2015 (apr): einde ICRm binnenlandse dienst</t>
+  </si>
+  <si>
+    <t>2017: ICRm(h?) in 1100</t>
+  </si>
+  <si>
+    <t>2018: ICR stammen 6 rijtuigen</t>
+  </si>
+  <si>
+    <t>2018 (aug): 9-rijtuigen stam extra</t>
+  </si>
+  <si>
+    <t>2019: 1x extra A-rijtuig per benelux stam</t>
+  </si>
+  <si>
+    <t>1986: tegenstrijdig benelux: HLE11+A+AB+BKD+B+B+Bs</t>
+  </si>
+  <si>
+    <t>1989: uitbreiding benelux extra rijtuig tot 7</t>
+  </si>
+  <si>
+    <t>2009: fyra over hsl</t>
+  </si>
+  <si>
+    <t>2005: inzet ICRm in vaste stammen</t>
+  </si>
+  <si>
+    <t>2007: fyra rijtuigen (in benelux). In verkeerde volgorde om naam niet te spoilen. Stam 7 rijtuigen</t>
+  </si>
+  <si>
+    <t>2014-2017: ICRmh 6- 7- 9-delige stammen voor hsl en benelux, zie railwiki</t>
+  </si>
+  <si>
+    <t>Consists obv foto's</t>
+  </si>
+  <si>
+    <t>ICR 5 1986</t>
+  </si>
+  <si>
+    <t>ICR 4 1985</t>
+  </si>
+  <si>
+    <t>ICR W 6 1988</t>
+  </si>
+  <si>
+    <t>Rijtuigen zo geflipt dat toilet rechts zit</t>
+  </si>
+  <si>
+    <t>ICR 5 1991</t>
+  </si>
+  <si>
+    <t>ICR 6 1994</t>
+  </si>
+  <si>
+    <t>ICR W 4 1991</t>
+  </si>
+  <si>
+    <t>ICR W 5 1993</t>
+  </si>
+  <si>
+    <t>ICR 4 1990</t>
+  </si>
+  <si>
+    <t>Lok</t>
+  </si>
+  <si>
+    <t>1100, 1200</t>
+  </si>
+  <si>
+    <t>Fyra rijtuigen geflipt dat ze allemaal achter elkaar kunnen. 1e klas vooraan (B, C).</t>
+  </si>
+  <si>
+    <t>HLE 11</t>
+  </si>
+  <si>
+    <t>ICRm Benelux 6 2007</t>
+  </si>
+  <si>
+    <t>ICRm Benelux 7 2009a</t>
+  </si>
+  <si>
+    <t>ICRm Benelux 7 2009b</t>
+  </si>
+  <si>
+    <t>TRAXX (NMBS)</t>
+  </si>
+  <si>
+    <t>ICRm Benelux 7 2009c</t>
+  </si>
+  <si>
+    <t>ICRm Benelux 7 2009d</t>
+  </si>
+  <si>
+    <t>TRAXX (Rood) + TRAXX (Rood)</t>
+  </si>
+  <si>
+    <t>ICRm TD7</t>
+  </si>
+  <si>
+    <t>ICRm TD9</t>
+  </si>
+  <si>
+    <t>ICRm Fyra 7 2009</t>
+  </si>
+  <si>
+    <t>ICRm Fyra 6 2011</t>
+  </si>
+  <si>
+    <t>TRAXX (Rood Fyra)</t>
+  </si>
+  <si>
+    <t>HLE 11, TRAXX (NMBS, voor Bs)</t>
+  </si>
+  <si>
+    <t>TRAXX (Rood Hispeed, voor Bs)</t>
+  </si>
+  <si>
+    <t>ICRm ICD 6 2014</t>
+  </si>
+  <si>
+    <t>TRAXX (NS)</t>
+  </si>
+  <si>
+    <t>ICR 4 1990 B</t>
+  </si>
+  <si>
+    <t>ICR 5 1990</t>
+  </si>
+  <si>
+    <t>ICR W 10 1993</t>
+  </si>
+  <si>
+    <t>ICR W 9 1993</t>
+  </si>
+  <si>
+    <t>ICR W F x 1993</t>
+  </si>
+  <si>
+    <t>ICR 7 1995</t>
+  </si>
+  <si>
+    <t>ICR 9 1995</t>
+  </si>
+  <si>
+    <t>? 95</t>
   </si>
 </sst>
 </file>
@@ -1270,16 +1734,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D39"/>
+  <dimension ref="A1:E106"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:D1"/>
+    <sheetView tabSelected="1" topLeftCell="A76" workbookViewId="0">
+      <selection activeCell="E87" sqref="E87"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
     <col min="1" max="1" width="2.6640625" customWidth="1"/>
-    <col min="2" max="2" width="16.33203125" style="4" customWidth="1"/>
+    <col min="2" max="2" width="20.265625" style="4" customWidth="1"/>
     <col min="3" max="3" width="9.19921875" style="4" customWidth="1"/>
   </cols>
   <sheetData>
@@ -1595,14 +2059,523 @@
         <v>41974</v>
       </c>
     </row>
-    <row r="37" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="37" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A37" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="39" spans="1:1" x14ac:dyDescent="0.45">
-      <c r="A39" t="s">
+    <row r="38" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A38" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="41" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A41" t="s">
         <v>24</v>
+      </c>
+    </row>
+    <row r="44" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A44" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="45" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="B45" s="4" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="46" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="B46" s="4" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="47" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="B47" s="4" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="48" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="B48" s="4" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="49" spans="2:2" x14ac:dyDescent="0.45">
+      <c r="B49" s="4" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="50" spans="2:2" x14ac:dyDescent="0.45">
+      <c r="B50" s="3" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="51" spans="2:2" x14ac:dyDescent="0.45">
+      <c r="B51" s="4" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="52" spans="2:2" x14ac:dyDescent="0.45">
+      <c r="B52" s="4" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="53" spans="2:2" x14ac:dyDescent="0.45">
+      <c r="B53" s="3" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="54" spans="2:2" x14ac:dyDescent="0.45">
+      <c r="B54" s="3" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="55" spans="2:2" x14ac:dyDescent="0.45">
+      <c r="B55" s="3" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="56" spans="2:2" x14ac:dyDescent="0.45">
+      <c r="B56" s="3" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="57" spans="2:2" x14ac:dyDescent="0.45">
+      <c r="B57" s="4" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="58" spans="2:2" x14ac:dyDescent="0.45">
+      <c r="B58" s="4" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="59" spans="2:2" x14ac:dyDescent="0.45">
+      <c r="B59" s="3" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="60" spans="2:2" x14ac:dyDescent="0.45">
+      <c r="B60" s="4" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="61" spans="2:2" x14ac:dyDescent="0.45">
+      <c r="B61" s="3" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="62" spans="2:2" x14ac:dyDescent="0.45">
+      <c r="B62" s="4" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="63" spans="2:2" x14ac:dyDescent="0.45">
+      <c r="B63" s="3" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="64" spans="2:2" x14ac:dyDescent="0.45">
+      <c r="B64" s="4" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="65" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="B65" s="3" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="66" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="B66" s="4" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="67" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="B67" s="4" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="68" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="B68" s="4" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="69" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="B69" s="4" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="70" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="B70" s="4" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="71" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="B71" s="4" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="77" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A77" t="s">
+        <v>87</v>
+      </c>
+      <c r="C77" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="D77" t="s">
+        <v>8</v>
+      </c>
+      <c r="E77" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="78" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="B78" s="4" t="s">
+        <v>89</v>
+      </c>
+      <c r="C78" s="4">
+        <v>31291</v>
+      </c>
+      <c r="D78" s="2">
+        <v>31291</v>
+      </c>
+      <c r="E78">
+        <v>1100</v>
+      </c>
+    </row>
+    <row r="79" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="B79" s="4" t="s">
+        <v>96</v>
+      </c>
+      <c r="C79" s="4">
+        <v>33055</v>
+      </c>
+      <c r="D79" s="4">
+        <v>35855</v>
+      </c>
+      <c r="E79">
+        <v>1100</v>
+      </c>
+    </row>
+    <row r="80" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="B80" s="4" t="s">
+        <v>117</v>
+      </c>
+      <c r="C80" s="4">
+        <v>33055</v>
+      </c>
+      <c r="D80" s="4">
+        <v>33055</v>
+      </c>
+      <c r="E80">
+        <v>1100</v>
+      </c>
+    </row>
+    <row r="81" spans="2:5" x14ac:dyDescent="0.45">
+      <c r="B81" s="4" t="s">
+        <v>88</v>
+      </c>
+      <c r="C81" s="4">
+        <v>31444</v>
+      </c>
+      <c r="D81" s="2">
+        <v>32994</v>
+      </c>
+      <c r="E81" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="82" spans="2:5" x14ac:dyDescent="0.45">
+      <c r="B82" s="4" t="s">
+        <v>118</v>
+      </c>
+      <c r="C82" s="4">
+        <v>33025</v>
+      </c>
+      <c r="D82" s="4">
+        <v>33025</v>
+      </c>
+      <c r="E82">
+        <v>1100</v>
+      </c>
+    </row>
+    <row r="83" spans="2:5" x14ac:dyDescent="0.45">
+      <c r="B83" s="4" t="s">
+        <v>92</v>
+      </c>
+      <c r="C83" s="4">
+        <v>33270</v>
+      </c>
+      <c r="D83" s="4">
+        <v>33270</v>
+      </c>
+      <c r="E83">
+        <v>1100</v>
+      </c>
+    </row>
+    <row r="84" spans="2:5" x14ac:dyDescent="0.45">
+      <c r="B84" s="4" t="s">
+        <v>93</v>
+      </c>
+      <c r="C84" s="4">
+        <v>34366</v>
+      </c>
+      <c r="D84" s="4">
+        <v>34366</v>
+      </c>
+      <c r="E84">
+        <v>1700</v>
+      </c>
+    </row>
+    <row r="85" spans="2:5" x14ac:dyDescent="0.45">
+      <c r="B85" s="4" t="s">
+        <v>122</v>
+      </c>
+      <c r="C85" s="4">
+        <v>34700</v>
+      </c>
+      <c r="D85" s="4">
+        <v>34700</v>
+      </c>
+      <c r="E85">
+        <v>1600</v>
+      </c>
+    </row>
+    <row r="86" spans="2:5" x14ac:dyDescent="0.45">
+      <c r="B86" s="4" t="s">
+        <v>123</v>
+      </c>
+      <c r="C86" s="4" t="s">
+        <v>124</v>
+      </c>
+      <c r="D86" s="4" t="s">
+        <v>124</v>
+      </c>
+      <c r="E86">
+        <v>1600</v>
+      </c>
+    </row>
+    <row r="87" spans="2:5" x14ac:dyDescent="0.45">
+      <c r="B87" s="4" t="s">
+        <v>94</v>
+      </c>
+      <c r="C87" s="4">
+        <v>33512</v>
+      </c>
+      <c r="D87" s="4">
+        <v>33512</v>
+      </c>
+      <c r="E87">
+        <v>1100</v>
+      </c>
+    </row>
+    <row r="88" spans="2:5" x14ac:dyDescent="0.45">
+      <c r="B88" s="4" t="s">
+        <v>95</v>
+      </c>
+      <c r="C88" s="4">
+        <v>34182</v>
+      </c>
+      <c r="D88" s="4">
+        <v>34182</v>
+      </c>
+      <c r="E88">
+        <v>1300</v>
+      </c>
+    </row>
+    <row r="89" spans="2:5" x14ac:dyDescent="0.45">
+      <c r="B89" s="4" t="s">
+        <v>90</v>
+      </c>
+      <c r="C89" s="4">
+        <v>32448</v>
+      </c>
+      <c r="D89" s="4">
+        <v>32448</v>
+      </c>
+      <c r="E89">
+        <v>1100</v>
+      </c>
+    </row>
+    <row r="90" spans="2:5" x14ac:dyDescent="0.45">
+      <c r="B90" s="4" t="s">
+        <v>120</v>
+      </c>
+      <c r="C90" s="4">
+        <v>34182</v>
+      </c>
+      <c r="D90" s="4">
+        <v>34182</v>
+      </c>
+      <c r="E90">
+        <v>1600</v>
+      </c>
+    </row>
+    <row r="91" spans="2:5" x14ac:dyDescent="0.45">
+      <c r="B91" s="4" t="s">
+        <v>119</v>
+      </c>
+      <c r="C91" s="4">
+        <v>34182</v>
+      </c>
+      <c r="D91" s="4">
+        <v>34182</v>
+      </c>
+      <c r="E91">
+        <v>1200</v>
+      </c>
+    </row>
+    <row r="92" spans="2:5" x14ac:dyDescent="0.45">
+      <c r="B92" s="4" t="s">
+        <v>121</v>
+      </c>
+      <c r="C92" s="4">
+        <v>34182</v>
+      </c>
+      <c r="D92" s="4">
+        <v>34182</v>
+      </c>
+      <c r="E92">
+        <v>1600</v>
+      </c>
+    </row>
+    <row r="94" spans="2:5" x14ac:dyDescent="0.45">
+      <c r="B94" s="4" t="s">
+        <v>108</v>
+      </c>
+      <c r="C94" s="4">
+        <v>39173</v>
+      </c>
+      <c r="D94" s="4">
+        <v>41913</v>
+      </c>
+      <c r="E94">
+        <v>1700</v>
+      </c>
+    </row>
+    <row r="95" spans="2:5" x14ac:dyDescent="0.45">
+      <c r="B95" s="4" t="s">
+        <v>109</v>
+      </c>
+      <c r="C95" s="4">
+        <v>39600</v>
+      </c>
+      <c r="D95" s="4">
+        <v>41699</v>
+      </c>
+      <c r="E95">
+        <v>1700</v>
+      </c>
+    </row>
+    <row r="97" spans="2:5" x14ac:dyDescent="0.45">
+      <c r="B97" s="4" t="s">
+        <v>101</v>
+      </c>
+      <c r="C97" s="4">
+        <v>39173</v>
+      </c>
+      <c r="D97" s="4">
+        <v>39173</v>
+      </c>
+      <c r="E97" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="98" spans="2:5" x14ac:dyDescent="0.45">
+      <c r="B98" s="4" t="s">
+        <v>102</v>
+      </c>
+      <c r="C98" s="4">
+        <v>40057</v>
+      </c>
+      <c r="D98" s="4">
+        <v>40057</v>
+      </c>
+      <c r="E98" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="99" spans="2:5" x14ac:dyDescent="0.45">
+      <c r="B99" s="4" t="s">
+        <v>103</v>
+      </c>
+      <c r="C99" s="4">
+        <v>39934</v>
+      </c>
+      <c r="D99" s="4">
+        <v>40179</v>
+      </c>
+      <c r="E99" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="100" spans="2:5" x14ac:dyDescent="0.45">
+      <c r="B100" s="4" t="s">
+        <v>105</v>
+      </c>
+      <c r="C100" s="4">
+        <v>40118</v>
+      </c>
+      <c r="D100" s="4">
+        <v>40118</v>
+      </c>
+      <c r="E100" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="101" spans="2:5" x14ac:dyDescent="0.45">
+      <c r="B101" s="4" t="s">
+        <v>106</v>
+      </c>
+      <c r="C101" s="4">
+        <v>40330</v>
+      </c>
+      <c r="D101" s="4">
+        <v>40330</v>
+      </c>
+      <c r="E101" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="103" spans="2:5" x14ac:dyDescent="0.45">
+      <c r="B103" s="4" t="s">
+        <v>111</v>
+      </c>
+      <c r="C103" s="4">
+        <v>40603</v>
+      </c>
+      <c r="D103" s="4">
+        <v>40603</v>
+      </c>
+      <c r="E103" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="104" spans="2:5" x14ac:dyDescent="0.45">
+      <c r="B104" s="4" t="s">
+        <v>110</v>
+      </c>
+      <c r="C104" s="4">
+        <v>40118</v>
+      </c>
+      <c r="D104" s="4">
+        <v>40118</v>
+      </c>
+      <c r="E104" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="106" spans="2:5" x14ac:dyDescent="0.45">
+      <c r="B106" s="4" t="s">
+        <v>115</v>
+      </c>
+      <c r="C106" s="4">
+        <v>41913</v>
+      </c>
+      <c r="D106" s="4">
+        <v>41913</v>
+      </c>
+      <c r="E106" t="s">
+        <v>116</v>
       </c>
     </row>
   </sheetData>
@@ -1614,10 +2587,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{34F6A220-FD91-4F5A-ACFA-A0D4B83AD909}">
-  <dimension ref="A1:D10"/>
+  <dimension ref="A1:D13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D19" sqref="D19"/>
+      <selection activeCell="A13" sqref="A13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -1737,6 +2710,11 @@
         <v>37956</v>
       </c>
     </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A13" t="s">
+        <v>91</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <legacyDrawing r:id="rId1"/>
@@ -1747,7 +2725,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C42AD58B-783D-4A65-88F6-4F4D48B1C5CA}">
   <dimension ref="A1:K32"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="E21" sqref="E21"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Research naar ICR combinaties
</commit_message>
<xml_diff>
--- a/RailWorks/Source/RailionLudmilla-Consists/Materieel/Rijtuigen/overzicht-inzet.xlsx
+++ b/RailWorks/Source/RailionLudmilla-Consists/Materieel/Rijtuigen/overzicht-inzet.xlsx
@@ -8,14 +8,15 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Games\Steam\steamapps\common\RailWorks\Source\RailionLudmilla-Consists\Materieel\Rijtuigen\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E385E382-57E2-424B-9445-86525F99945D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{97DD62F6-A0B7-4500-B9ED-200E04D1CD23}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="14400" windowHeight="15600" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-98" yWindow="-98" windowWidth="28996" windowHeight="15796" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="ICR" sheetId="1" r:id="rId1"/>
-    <sheet name="Plan W" sheetId="2" r:id="rId2"/>
-    <sheet name="DDM1" sheetId="3" r:id="rId3"/>
+    <sheet name="ICR Chaos of Getrokken treinen" sheetId="5" r:id="rId2"/>
+    <sheet name="Plan W" sheetId="2" r:id="rId3"/>
+    <sheet name="DDM1" sheetId="3" r:id="rId4"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -456,7 +457,7 @@
     <author>Tom</author>
   </authors>
   <commentList>
-    <comment ref="A1" authorId="0" shapeId="0" xr:uid="{CEE0F991-71E5-4E1F-A35A-85DBA5145ADA}">
+    <comment ref="A1" authorId="0" shapeId="0" xr:uid="{31D5E7F7-20F9-4587-9096-373BD8B3695B}">
       <text>
         <r>
           <rPr>
@@ -464,7 +465,7 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
-            <charset val="1"/>
+            <family val="2"/>
           </rPr>
           <t>Tom:</t>
         </r>
@@ -473,15 +474,15 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
-            <charset val="1"/>
+            <family val="2"/>
           </rPr>
           <t xml:space="preserve">
-W1: nummer eindigt op 4xx
-W2: nummer eindigt op 5xx</t>
+Voorstel naamgeving:
+ICR_&lt;IC|ICplus|Bnl|HSL&gt;_&lt;lengte|TDx&gt;_&lt;eerste&gt;_&lt;laatste&gt;.xml</t>
         </r>
       </text>
     </comment>
-    <comment ref="A2" authorId="0" shapeId="0" xr:uid="{5B3E9958-933D-4EE5-A4B3-39384BEC44DE}">
+    <comment ref="A3" authorId="0" shapeId="0" xr:uid="{C4B1F1DD-00F9-4BB3-8EE6-BC6711DDCD00}">
       <text>
         <r>
           <rPr>
@@ -489,7 +490,7 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
-            <charset val="1"/>
+            <family val="2"/>
           </rPr>
           <t>Tom:</t>
         </r>
@@ -498,14 +499,14 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
-            <charset val="1"/>
+            <family val="2"/>
           </rPr>
           <t xml:space="preserve">
-slechts 3 rijtuigen, rest was Bnl</t>
+Super chaotisch. Ga er vanuit dat alles wat beschikbaar was wel eens in combinatie voorkwam</t>
         </r>
       </text>
     </comment>
-    <comment ref="A3" authorId="0" shapeId="0" xr:uid="{085F7D9D-C4DD-425B-A842-64C7444DE888}">
+    <comment ref="AD16" authorId="0" shapeId="0" xr:uid="{C32AD2E1-D3CD-4B24-82E4-08A056D33FD2}">
       <text>
         <r>
           <rPr>
@@ -513,7 +514,7 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
-            <charset val="1"/>
+            <family val="2"/>
           </rPr>
           <t>Tom:</t>
         </r>
@@ -522,14 +523,14 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
-            <charset val="1"/>
+            <family val="2"/>
           </rPr>
           <t xml:space="preserve">
-'73 op railwiki</t>
+AB</t>
         </r>
       </text>
     </comment>
-    <comment ref="A4" authorId="0" shapeId="0" xr:uid="{A7122EB4-7A95-4183-AD1A-07E1EE6C9FAC}">
+    <comment ref="A26" authorId="0" shapeId="0" xr:uid="{1E6CB8B5-2748-4BFB-8F1A-E31966865A3F}">
       <text>
         <r>
           <rPr>
@@ -537,7 +538,7 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
-            <charset val="1"/>
+            <family val="2"/>
           </rPr>
           <t>Tom:</t>
         </r>
@@ -546,107 +547,10 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
-            <charset val="1"/>
+            <family val="2"/>
           </rPr>
           <t xml:space="preserve">
-andere ramen</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="C6" authorId="0" shapeId="0" xr:uid="{5398D912-08D9-42BF-86E7-7BAE2EA846B2}">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <charset val="1"/>
-          </rPr>
-          <t>Tom:</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <charset val="1"/>
-          </rPr>
-          <t xml:space="preserve">
-herindienststelling</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="A8" authorId="0" shapeId="0" xr:uid="{DFF8A1D1-7519-4195-B8F9-E5EC95FCCEA3}">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <charset val="1"/>
-          </rPr>
-          <t>Tom:</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <charset val="1"/>
-          </rPr>
-          <t xml:space="preserve">
-blauw met gele deuren
-enkel rijtuig: 507</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="A9" authorId="0" shapeId="0" xr:uid="{4D199028-542A-4062-A684-51D377355B62}">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <charset val="1"/>
-          </rPr>
-          <t>Tom:</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <charset val="1"/>
-          </rPr>
-          <t xml:space="preserve">
-herkenbaar aan nummer rechts ipv midden</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="C10" authorId="0" shapeId="0" xr:uid="{4EBA6DD3-4035-4F4E-8B87-BF9290307E8A}">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <charset val="1"/>
-          </rPr>
-          <t>Tom:</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <charset val="1"/>
-          </rPr>
-          <t xml:space="preserve">
-herindienststelling</t>
+Bvk als rijtuig</t>
         </r>
       </text>
     </comment>
@@ -660,6 +564,210 @@
     <author>Tom</author>
   </authors>
   <commentList>
+    <comment ref="A1" authorId="0" shapeId="0" xr:uid="{CEE0F991-71E5-4E1F-A35A-85DBA5145ADA}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Tom:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+W1: nummer eindigt op 4xx
+W2: nummer eindigt op 5xx</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="A2" authorId="0" shapeId="0" xr:uid="{5B3E9958-933D-4EE5-A4B3-39384BEC44DE}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Tom:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+slechts 3 rijtuigen, rest was Bnl</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="A3" authorId="0" shapeId="0" xr:uid="{085F7D9D-C4DD-425B-A842-64C7444DE888}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Tom:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+'73 op railwiki</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="A4" authorId="0" shapeId="0" xr:uid="{A7122EB4-7A95-4183-AD1A-07E1EE6C9FAC}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Tom:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+andere ramen</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="C6" authorId="0" shapeId="0" xr:uid="{5398D912-08D9-42BF-86E7-7BAE2EA846B2}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Tom:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+herindienststelling</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="A8" authorId="0" shapeId="0" xr:uid="{DFF8A1D1-7519-4195-B8F9-E5EC95FCCEA3}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Tom:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+blauw met gele deuren
+enkel rijtuig: 507</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="A9" authorId="0" shapeId="0" xr:uid="{4D199028-542A-4062-A684-51D377355B62}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Tom:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+herkenbaar aan nummer rechts ipv midden</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="C10" authorId="0" shapeId="0" xr:uid="{4EBA6DD3-4035-4F4E-8B87-BF9290307E8A}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Tom:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+herindienststelling</t>
+        </r>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
+<file path=xl/comments4.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
+  <authors>
+    <author>Tom</author>
+  </authors>
+  <commentList>
     <comment ref="E8" authorId="0" shapeId="0" xr:uid="{7A3C02EA-EF21-4F8D-8D86-BAF1B29EA7C7}">
       <text>
         <r>
@@ -1001,7 +1109,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="165" uniqueCount="125">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="633" uniqueCount="165">
   <si>
     <t>ICR benelux</t>
   </si>
@@ -1376,6 +1484,126 @@
   </si>
   <si>
     <t>? 95</t>
+  </si>
+  <si>
+    <t>ICR IC</t>
+  </si>
+  <si>
+    <t>ICR Bnl</t>
+  </si>
+  <si>
+    <t>ICR IC+</t>
+  </si>
+  <si>
+    <t>Intercity</t>
+  </si>
+  <si>
+    <t>DD-AR Bvk</t>
+  </si>
+  <si>
+    <t>K4</t>
+  </si>
+  <si>
+    <t>M2</t>
+  </si>
+  <si>
+    <t>ICK</t>
+  </si>
+  <si>
+    <t>ICL</t>
+  </si>
+  <si>
+    <t>ICRm IC</t>
+  </si>
+  <si>
+    <t>ICRm BDs</t>
+  </si>
+  <si>
+    <t>ICRm Bnl</t>
+  </si>
+  <si>
+    <t>ICR Bnl Bs</t>
+  </si>
+  <si>
+    <t>1x DDM-1 Bv</t>
+  </si>
+  <si>
+    <t>Plan W</t>
+  </si>
+  <si>
+    <t>Plan Fiets</t>
+  </si>
+  <si>
+    <t>Plan E</t>
+  </si>
+  <si>
+    <t>Stalen D</t>
+  </si>
+  <si>
+    <t>1800</t>
+  </si>
+  <si>
+    <t>Benelux</t>
+  </si>
+  <si>
+    <t>ICRm IC BDs</t>
+  </si>
+  <si>
+    <t>IC+</t>
+  </si>
+  <si>
+    <t>1700 sandwich</t>
+  </si>
+  <si>
+    <t>DB Am/Bm</t>
+  </si>
+  <si>
+    <t>DB IR</t>
+  </si>
+  <si>
+    <t>ICRm TD-7</t>
+  </si>
+  <si>
+    <t>ICRm TD-10</t>
+  </si>
+  <si>
+    <t>DDM-1 Bvk + Bv</t>
+  </si>
+  <si>
+    <t>ICRm Fyra mix</t>
+  </si>
+  <si>
+    <t>ICRm Fyra op volgorde</t>
+  </si>
+  <si>
+    <t>1x TRAXX</t>
+  </si>
+  <si>
+    <t>2x TRAXX</t>
+  </si>
+  <si>
+    <t>1800 sandwich</t>
+  </si>
+  <si>
+    <t>ICRm Fyra met logo</t>
+  </si>
+  <si>
+    <t>ICR Fyra Bs</t>
+  </si>
+  <si>
+    <t>ICRm IC?</t>
+  </si>
+  <si>
+    <t>?</t>
+  </si>
+  <si>
+    <t>ICRm TD-9</t>
+  </si>
+  <si>
+    <t>Fyra / ICD</t>
+  </si>
+  <si>
+    <t>&gt;1x DDM-1 Bv</t>
   </si>
 </sst>
 </file>
@@ -1428,12 +1656,18 @@
       <charset val="1"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -1448,12 +1682,22 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="17" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="164" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment textRotation="90"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Standaard" xfId="0" builtinId="0"/>
@@ -1734,10 +1978,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E106"/>
+  <dimension ref="A1:XFD142"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A76" workbookViewId="0">
-      <selection activeCell="E87" sqref="E87"/>
+    <sheetView topLeftCell="A43" workbookViewId="0">
+      <selection activeCell="E130" sqref="E130"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -2578,6 +2822,88 @@
         <v>116</v>
       </c>
     </row>
+    <row r="114" spans="4:4" x14ac:dyDescent="0.45">
+      <c r="D114" s="4"/>
+    </row>
+    <row r="115" spans="4:4" x14ac:dyDescent="0.45">
+      <c r="D115" s="4"/>
+    </row>
+    <row r="116" spans="4:4" x14ac:dyDescent="0.45">
+      <c r="D116" s="4"/>
+    </row>
+    <row r="117" spans="4:4" x14ac:dyDescent="0.45">
+      <c r="D117" s="4"/>
+    </row>
+    <row r="118" spans="4:4" x14ac:dyDescent="0.45">
+      <c r="D118" s="4"/>
+    </row>
+    <row r="119" spans="4:4" x14ac:dyDescent="0.45">
+      <c r="D119" s="4"/>
+    </row>
+    <row r="120" spans="4:4" x14ac:dyDescent="0.45">
+      <c r="D120" s="4"/>
+    </row>
+    <row r="121" spans="4:4" x14ac:dyDescent="0.45">
+      <c r="D121" s="4"/>
+    </row>
+    <row r="122" spans="4:4" x14ac:dyDescent="0.45">
+      <c r="D122" s="4"/>
+    </row>
+    <row r="123" spans="4:4" x14ac:dyDescent="0.45">
+      <c r="D123" s="4"/>
+    </row>
+    <row r="124" spans="4:4" x14ac:dyDescent="0.45">
+      <c r="D124" s="4"/>
+    </row>
+    <row r="125" spans="4:4" x14ac:dyDescent="0.45">
+      <c r="D125" s="4"/>
+    </row>
+    <row r="126" spans="4:4" x14ac:dyDescent="0.45">
+      <c r="D126" s="4"/>
+    </row>
+    <row r="127" spans="4:4" x14ac:dyDescent="0.45">
+      <c r="D127" s="4"/>
+    </row>
+    <row r="128" spans="4:4" x14ac:dyDescent="0.45">
+      <c r="D128" s="4"/>
+    </row>
+    <row r="129" spans="4:4 16384:16384" x14ac:dyDescent="0.45">
+      <c r="D129" s="4"/>
+    </row>
+    <row r="130" spans="4:4 16384:16384" x14ac:dyDescent="0.45">
+      <c r="D130" s="4"/>
+    </row>
+    <row r="131" spans="4:4 16384:16384" x14ac:dyDescent="0.45">
+      <c r="D131" s="4"/>
+    </row>
+    <row r="132" spans="4:4 16384:16384" x14ac:dyDescent="0.45">
+      <c r="D132" s="4"/>
+    </row>
+    <row r="133" spans="4:4 16384:16384" x14ac:dyDescent="0.45">
+      <c r="D133" s="4"/>
+    </row>
+    <row r="134" spans="4:4 16384:16384" x14ac:dyDescent="0.45">
+      <c r="D134" s="4"/>
+    </row>
+    <row r="135" spans="4:4 16384:16384" x14ac:dyDescent="0.45">
+      <c r="D135" s="4"/>
+    </row>
+    <row r="136" spans="4:4 16384:16384" x14ac:dyDescent="0.45">
+      <c r="D136" s="4"/>
+    </row>
+    <row r="137" spans="4:4 16384:16384" x14ac:dyDescent="0.45">
+      <c r="D137" s="4"/>
+    </row>
+    <row r="140" spans="4:4 16384:16384" x14ac:dyDescent="0.45">
+      <c r="D140" s="4"/>
+      <c r="XFD140" s="4"/>
+    </row>
+    <row r="141" spans="4:4 16384:16384" x14ac:dyDescent="0.45">
+      <c r="D141" s="4"/>
+    </row>
+    <row r="142" spans="4:4 16384:16384" x14ac:dyDescent="0.45">
+      <c r="D142" s="4"/>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>
@@ -2586,6 +2912,1816 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{ED6AB4D6-199D-4730-8D3B-777B771D0456}">
+  <dimension ref="A1:AW68"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane xSplit="1" ySplit="2" topLeftCell="B3" activePane="bottomRight" state="frozen"/>
+      <selection pane="topRight" activeCell="B1" sqref="B1"/>
+      <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
+      <selection pane="bottomRight" activeCell="X19" sqref="X19"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <cols>
+    <col min="1" max="1" width="18.46484375" customWidth="1"/>
+    <col min="2" max="6" width="2.59765625" style="9" customWidth="1"/>
+    <col min="7" max="49" width="2.59765625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:49" ht="15" x14ac:dyDescent="0.45">
+      <c r="B1" s="8">
+        <v>76</v>
+      </c>
+      <c r="C1" s="8">
+        <v>77</v>
+      </c>
+      <c r="D1" s="8">
+        <v>78</v>
+      </c>
+      <c r="E1" s="8">
+        <v>79</v>
+      </c>
+      <c r="F1" s="8">
+        <v>80</v>
+      </c>
+      <c r="G1" s="5">
+        <v>81</v>
+      </c>
+      <c r="H1" s="5">
+        <v>82</v>
+      </c>
+      <c r="I1" s="5">
+        <v>83</v>
+      </c>
+      <c r="J1" s="5">
+        <v>84</v>
+      </c>
+      <c r="K1" s="5">
+        <v>85</v>
+      </c>
+      <c r="L1" s="5">
+        <v>86</v>
+      </c>
+      <c r="M1" s="5">
+        <v>87</v>
+      </c>
+      <c r="N1" s="5">
+        <v>88</v>
+      </c>
+      <c r="O1" s="5">
+        <v>89</v>
+      </c>
+      <c r="P1" s="5">
+        <v>90</v>
+      </c>
+      <c r="Q1" s="5">
+        <v>91</v>
+      </c>
+      <c r="R1" s="5">
+        <v>92</v>
+      </c>
+      <c r="S1" s="5">
+        <v>93</v>
+      </c>
+      <c r="T1" s="5">
+        <v>94</v>
+      </c>
+      <c r="U1" s="5">
+        <v>95</v>
+      </c>
+      <c r="V1" s="5">
+        <v>96</v>
+      </c>
+      <c r="W1" s="5">
+        <v>97</v>
+      </c>
+      <c r="X1" s="5">
+        <v>98</v>
+      </c>
+      <c r="Y1" s="5">
+        <v>99</v>
+      </c>
+      <c r="Z1" s="5">
+        <v>0</v>
+      </c>
+      <c r="AA1" s="5">
+        <v>1</v>
+      </c>
+      <c r="AB1" s="5">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2" spans="1:49" ht="15" x14ac:dyDescent="0.45">
+      <c r="B2" s="8">
+        <v>75</v>
+      </c>
+      <c r="C2" s="8">
+        <v>76</v>
+      </c>
+      <c r="D2" s="8">
+        <v>77</v>
+      </c>
+      <c r="E2" s="8">
+        <v>78</v>
+      </c>
+      <c r="F2" s="8">
+        <v>79</v>
+      </c>
+      <c r="G2" s="5">
+        <v>80</v>
+      </c>
+      <c r="H2" s="5">
+        <v>81</v>
+      </c>
+      <c r="I2" s="5">
+        <v>82</v>
+      </c>
+      <c r="J2" s="5">
+        <v>83</v>
+      </c>
+      <c r="K2" s="5">
+        <v>84</v>
+      </c>
+      <c r="L2" s="5">
+        <v>85</v>
+      </c>
+      <c r="M2" s="5">
+        <v>86</v>
+      </c>
+      <c r="N2" s="5">
+        <v>87</v>
+      </c>
+      <c r="O2" s="5">
+        <v>88</v>
+      </c>
+      <c r="P2" s="5">
+        <v>89</v>
+      </c>
+      <c r="Q2" s="5">
+        <v>90</v>
+      </c>
+      <c r="R2" s="5">
+        <v>91</v>
+      </c>
+      <c r="S2" s="5">
+        <v>92</v>
+      </c>
+      <c r="T2" s="5">
+        <v>93</v>
+      </c>
+      <c r="U2" s="5">
+        <v>94</v>
+      </c>
+      <c r="V2" s="5">
+        <v>95</v>
+      </c>
+      <c r="W2" s="5">
+        <v>96</v>
+      </c>
+      <c r="X2" s="5">
+        <v>97</v>
+      </c>
+      <c r="Y2" s="5">
+        <v>98</v>
+      </c>
+      <c r="Z2" s="5">
+        <v>99</v>
+      </c>
+      <c r="AA2" s="5">
+        <v>0</v>
+      </c>
+      <c r="AB2" s="5">
+        <v>1</v>
+      </c>
+      <c r="AC2" s="5">
+        <v>3</v>
+      </c>
+      <c r="AD2" s="5">
+        <v>4</v>
+      </c>
+      <c r="AE2" s="5">
+        <v>5</v>
+      </c>
+      <c r="AF2" s="5">
+        <v>6</v>
+      </c>
+      <c r="AG2" s="5">
+        <v>7</v>
+      </c>
+      <c r="AH2" s="5">
+        <v>8</v>
+      </c>
+      <c r="AI2" s="5">
+        <v>9</v>
+      </c>
+      <c r="AJ2" s="5">
+        <v>10</v>
+      </c>
+      <c r="AK2" s="5">
+        <v>11</v>
+      </c>
+      <c r="AL2" s="5">
+        <v>12</v>
+      </c>
+      <c r="AM2" s="5">
+        <v>13</v>
+      </c>
+      <c r="AN2" s="5">
+        <v>14</v>
+      </c>
+      <c r="AO2" s="5">
+        <v>15</v>
+      </c>
+      <c r="AP2" s="5">
+        <v>16</v>
+      </c>
+      <c r="AQ2" s="5">
+        <v>17</v>
+      </c>
+      <c r="AR2" s="5">
+        <v>18</v>
+      </c>
+      <c r="AS2" s="5">
+        <v>19</v>
+      </c>
+      <c r="AT2" s="5">
+        <v>20</v>
+      </c>
+      <c r="AU2" s="5">
+        <v>21</v>
+      </c>
+      <c r="AV2" s="5">
+        <v>22</v>
+      </c>
+      <c r="AW2" s="5">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="3" spans="1:49" x14ac:dyDescent="0.45">
+      <c r="A3" s="1" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="4" spans="1:49" x14ac:dyDescent="0.45">
+      <c r="A4" s="6">
+        <v>1100</v>
+      </c>
+      <c r="G4" t="s">
+        <v>161</v>
+      </c>
+      <c r="H4" t="s">
+        <v>44</v>
+      </c>
+      <c r="I4" t="s">
+        <v>161</v>
+      </c>
+      <c r="J4" t="s">
+        <v>44</v>
+      </c>
+      <c r="K4" t="s">
+        <v>44</v>
+      </c>
+      <c r="L4" t="s">
+        <v>44</v>
+      </c>
+      <c r="M4" t="s">
+        <v>44</v>
+      </c>
+      <c r="N4" t="s">
+        <v>161</v>
+      </c>
+      <c r="O4" t="s">
+        <v>44</v>
+      </c>
+      <c r="P4" t="s">
+        <v>44</v>
+      </c>
+      <c r="Q4" t="s">
+        <v>44</v>
+      </c>
+      <c r="R4" t="s">
+        <v>44</v>
+      </c>
+      <c r="S4" t="s">
+        <v>44</v>
+      </c>
+      <c r="T4" t="s">
+        <v>44</v>
+      </c>
+      <c r="U4" t="s">
+        <v>161</v>
+      </c>
+      <c r="V4" t="s">
+        <v>161</v>
+      </c>
+      <c r="W4" t="s">
+        <v>44</v>
+      </c>
+      <c r="X4" t="s">
+        <v>161</v>
+      </c>
+      <c r="Y4" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="5" spans="1:49" x14ac:dyDescent="0.45">
+      <c r="A5" s="6">
+        <v>1200</v>
+      </c>
+      <c r="J5" t="s">
+        <v>44</v>
+      </c>
+      <c r="K5" t="s">
+        <v>161</v>
+      </c>
+      <c r="L5" t="s">
+        <v>161</v>
+      </c>
+      <c r="M5" t="s">
+        <v>44</v>
+      </c>
+      <c r="N5" t="s">
+        <v>44</v>
+      </c>
+      <c r="O5" t="s">
+        <v>44</v>
+      </c>
+      <c r="P5" t="s">
+        <v>44</v>
+      </c>
+      <c r="Q5" t="s">
+        <v>44</v>
+      </c>
+      <c r="R5" t="s">
+        <v>44</v>
+      </c>
+      <c r="S5" t="s">
+        <v>44</v>
+      </c>
+      <c r="T5" t="s">
+        <v>44</v>
+      </c>
+      <c r="U5" t="s">
+        <v>44</v>
+      </c>
+      <c r="V5" t="s">
+        <v>161</v>
+      </c>
+      <c r="W5" t="s">
+        <v>161</v>
+      </c>
+      <c r="X5" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="6" spans="1:49" x14ac:dyDescent="0.45">
+      <c r="A6" s="6">
+        <v>1300</v>
+      </c>
+      <c r="K6" t="s">
+        <v>44</v>
+      </c>
+      <c r="L6" t="s">
+        <v>161</v>
+      </c>
+      <c r="M6" t="s">
+        <v>161</v>
+      </c>
+      <c r="N6" t="s">
+        <v>161</v>
+      </c>
+      <c r="O6" t="s">
+        <v>161</v>
+      </c>
+      <c r="P6" t="s">
+        <v>161</v>
+      </c>
+      <c r="Q6" t="s">
+        <v>44</v>
+      </c>
+      <c r="R6" t="s">
+        <v>44</v>
+      </c>
+      <c r="S6" t="s">
+        <v>44</v>
+      </c>
+      <c r="T6" t="s">
+        <v>161</v>
+      </c>
+      <c r="U6" t="s">
+        <v>161</v>
+      </c>
+      <c r="V6" t="s">
+        <v>44</v>
+      </c>
+      <c r="W6" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="7" spans="1:49" x14ac:dyDescent="0.45">
+      <c r="A7" s="6">
+        <v>1500</v>
+      </c>
+      <c r="G7" t="s">
+        <v>161</v>
+      </c>
+      <c r="H7" t="s">
+        <v>44</v>
+      </c>
+      <c r="I7" t="s">
+        <v>161</v>
+      </c>
+      <c r="J7" t="s">
+        <v>44</v>
+      </c>
+      <c r="K7" t="s">
+        <v>44</v>
+      </c>
+      <c r="L7" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="8" spans="1:49" x14ac:dyDescent="0.45">
+      <c r="A8" s="6">
+        <v>1600</v>
+      </c>
+      <c r="H8" t="s">
+        <v>44</v>
+      </c>
+      <c r="I8" t="s">
+        <v>44</v>
+      </c>
+      <c r="J8" t="s">
+        <v>161</v>
+      </c>
+      <c r="K8" t="s">
+        <v>161</v>
+      </c>
+      <c r="L8" t="s">
+        <v>44</v>
+      </c>
+      <c r="M8" t="s">
+        <v>161</v>
+      </c>
+      <c r="N8" t="s">
+        <v>161</v>
+      </c>
+      <c r="O8" t="s">
+        <v>161</v>
+      </c>
+      <c r="P8" t="s">
+        <v>44</v>
+      </c>
+      <c r="Q8" t="s">
+        <v>44</v>
+      </c>
+      <c r="R8" t="s">
+        <v>44</v>
+      </c>
+      <c r="S8" t="s">
+        <v>161</v>
+      </c>
+      <c r="T8" t="s">
+        <v>161</v>
+      </c>
+      <c r="U8" t="s">
+        <v>44</v>
+      </c>
+      <c r="V8" t="s">
+        <v>44</v>
+      </c>
+      <c r="W8" t="s">
+        <v>44</v>
+      </c>
+      <c r="X8" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="9" spans="1:49" x14ac:dyDescent="0.45">
+      <c r="A9" s="6">
+        <v>1700</v>
+      </c>
+      <c r="X9" t="s">
+        <v>44</v>
+      </c>
+      <c r="Y9" t="s">
+        <v>44</v>
+      </c>
+      <c r="Z9" t="s">
+        <v>161</v>
+      </c>
+      <c r="AA9" t="s">
+        <v>44</v>
+      </c>
+      <c r="AB9" t="s">
+        <v>44</v>
+      </c>
+      <c r="AC9" t="s">
+        <v>44</v>
+      </c>
+      <c r="AD9" t="s">
+        <v>44</v>
+      </c>
+      <c r="AE9" t="s">
+        <v>44</v>
+      </c>
+      <c r="AF9" t="s">
+        <v>161</v>
+      </c>
+      <c r="AG9" t="s">
+        <v>44</v>
+      </c>
+      <c r="AH9" t="s">
+        <v>44</v>
+      </c>
+      <c r="AI9" t="s">
+        <v>44</v>
+      </c>
+      <c r="AJ9" t="s">
+        <v>44</v>
+      </c>
+      <c r="AK9" t="s">
+        <v>161</v>
+      </c>
+      <c r="AL9" t="s">
+        <v>44</v>
+      </c>
+      <c r="AM9" t="s">
+        <v>44</v>
+      </c>
+      <c r="AN9" t="s">
+        <v>44</v>
+      </c>
+      <c r="AO9" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="10" spans="1:49" x14ac:dyDescent="0.45">
+      <c r="A10" s="6" t="s">
+        <v>147</v>
+      </c>
+      <c r="Z10" t="s">
+        <v>44</v>
+      </c>
+      <c r="AA10" t="s">
+        <v>161</v>
+      </c>
+      <c r="AB10" t="s">
+        <v>44</v>
+      </c>
+      <c r="AC10" t="s">
+        <v>161</v>
+      </c>
+      <c r="AD10" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="11" spans="1:49" x14ac:dyDescent="0.45">
+      <c r="A11" s="6" t="s">
+        <v>143</v>
+      </c>
+      <c r="Y11" t="s">
+        <v>44</v>
+      </c>
+      <c r="Z11" t="s">
+        <v>44</v>
+      </c>
+      <c r="AA11" t="s">
+        <v>44</v>
+      </c>
+      <c r="AB11" t="s">
+        <v>44</v>
+      </c>
+      <c r="AC11" t="s">
+        <v>44</v>
+      </c>
+      <c r="AD11" t="s">
+        <v>44</v>
+      </c>
+      <c r="AE11" t="s">
+        <v>161</v>
+      </c>
+      <c r="AF11" t="s">
+        <v>161</v>
+      </c>
+      <c r="AG11" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="12" spans="1:49" x14ac:dyDescent="0.45">
+      <c r="A12" s="6" t="s">
+        <v>157</v>
+      </c>
+      <c r="AG12" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="13" spans="1:49" x14ac:dyDescent="0.45">
+      <c r="A13" s="6" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="14" spans="1:49" x14ac:dyDescent="0.45">
+      <c r="A14" s="6" t="s">
+        <v>156</v>
+      </c>
+      <c r="AQ14" t="s">
+        <v>44</v>
+      </c>
+      <c r="AR14" t="s">
+        <v>44</v>
+      </c>
+      <c r="AS14" t="s">
+        <v>44</v>
+      </c>
+      <c r="AT14" t="s">
+        <v>161</v>
+      </c>
+      <c r="AU14" t="s">
+        <v>44</v>
+      </c>
+      <c r="AV14" t="s">
+        <v>44</v>
+      </c>
+      <c r="AW14" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="15" spans="1:49" x14ac:dyDescent="0.45">
+      <c r="A15" t="s">
+        <v>125</v>
+      </c>
+      <c r="G15" t="s">
+        <v>44</v>
+      </c>
+      <c r="H15" t="s">
+        <v>44</v>
+      </c>
+      <c r="I15" t="s">
+        <v>44</v>
+      </c>
+      <c r="J15" t="s">
+        <v>44</v>
+      </c>
+      <c r="K15" t="s">
+        <v>44</v>
+      </c>
+      <c r="L15" t="s">
+        <v>44</v>
+      </c>
+      <c r="M15" t="s">
+        <v>44</v>
+      </c>
+      <c r="N15" t="s">
+        <v>44</v>
+      </c>
+      <c r="O15" t="s">
+        <v>44</v>
+      </c>
+      <c r="P15" t="s">
+        <v>44</v>
+      </c>
+      <c r="Q15" t="s">
+        <v>44</v>
+      </c>
+      <c r="R15" t="s">
+        <v>44</v>
+      </c>
+      <c r="S15" t="s">
+        <v>44</v>
+      </c>
+      <c r="T15" t="s">
+        <v>44</v>
+      </c>
+      <c r="U15" t="s">
+        <v>44</v>
+      </c>
+      <c r="V15" t="s">
+        <v>44</v>
+      </c>
+      <c r="W15" t="s">
+        <v>44</v>
+      </c>
+      <c r="X15" t="s">
+        <v>44</v>
+      </c>
+      <c r="Y15" t="s">
+        <v>44</v>
+      </c>
+      <c r="Z15" t="s">
+        <v>44</v>
+      </c>
+      <c r="AA15" t="s">
+        <v>44</v>
+      </c>
+      <c r="AB15" t="s">
+        <v>44</v>
+      </c>
+      <c r="AC15" t="s">
+        <v>44</v>
+      </c>
+      <c r="AD15" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="16" spans="1:49" x14ac:dyDescent="0.45">
+      <c r="A16" t="s">
+        <v>126</v>
+      </c>
+      <c r="O16" t="s">
+        <v>44</v>
+      </c>
+      <c r="P16" t="s">
+        <v>44</v>
+      </c>
+      <c r="AB16" t="s">
+        <v>44</v>
+      </c>
+      <c r="AC16" t="s">
+        <v>44</v>
+      </c>
+      <c r="AD16" t="s">
+        <v>44</v>
+      </c>
+      <c r="AE16" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="17" spans="1:49" x14ac:dyDescent="0.45">
+      <c r="A17" t="s">
+        <v>134</v>
+      </c>
+      <c r="AB17" t="s">
+        <v>44</v>
+      </c>
+      <c r="AC17" t="s">
+        <v>44</v>
+      </c>
+      <c r="AD17" t="s">
+        <v>44</v>
+      </c>
+      <c r="AE17" t="s">
+        <v>44</v>
+      </c>
+      <c r="AF17" t="s">
+        <v>44</v>
+      </c>
+      <c r="AG17" s="10"/>
+      <c r="AH17" s="10"/>
+      <c r="AI17" s="10"/>
+    </row>
+    <row r="18" spans="1:49" x14ac:dyDescent="0.45">
+      <c r="A18" t="s">
+        <v>135</v>
+      </c>
+      <c r="AD18" t="s">
+        <v>44</v>
+      </c>
+      <c r="AE18" t="s">
+        <v>44</v>
+      </c>
+      <c r="AF18" t="s">
+        <v>44</v>
+      </c>
+      <c r="AG18" s="10"/>
+      <c r="AH18" s="10"/>
+      <c r="AI18" s="10"/>
+    </row>
+    <row r="19" spans="1:49" x14ac:dyDescent="0.45">
+      <c r="A19" t="s">
+        <v>136</v>
+      </c>
+      <c r="AB19" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="20" spans="1:49" x14ac:dyDescent="0.45">
+      <c r="A20" t="s">
+        <v>150</v>
+      </c>
+      <c r="AG20" t="s">
+        <v>44</v>
+      </c>
+      <c r="AH20" t="s">
+        <v>44</v>
+      </c>
+      <c r="AI20" t="s">
+        <v>44</v>
+      </c>
+      <c r="AJ20" t="s">
+        <v>161</v>
+      </c>
+      <c r="AK20" t="s">
+        <v>161</v>
+      </c>
+      <c r="AL20" t="s">
+        <v>44</v>
+      </c>
+      <c r="AM20" t="s">
+        <v>44</v>
+      </c>
+      <c r="AN20" t="s">
+        <v>44</v>
+      </c>
+      <c r="AO20" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="21" spans="1:49" x14ac:dyDescent="0.45">
+      <c r="A21" t="s">
+        <v>162</v>
+      </c>
+      <c r="AN21" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="22" spans="1:49" x14ac:dyDescent="0.45">
+      <c r="A22" t="s">
+        <v>151</v>
+      </c>
+      <c r="AG22" t="s">
+        <v>44</v>
+      </c>
+      <c r="AH22" t="s">
+        <v>44</v>
+      </c>
+      <c r="AI22" t="s">
+        <v>44</v>
+      </c>
+      <c r="AJ22" t="s">
+        <v>44</v>
+      </c>
+      <c r="AK22" t="s">
+        <v>161</v>
+      </c>
+      <c r="AL22" t="s">
+        <v>44</v>
+      </c>
+      <c r="AM22" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="23" spans="1:49" x14ac:dyDescent="0.45">
+      <c r="A23" t="s">
+        <v>22</v>
+      </c>
+      <c r="AQ23" t="s">
+        <v>44</v>
+      </c>
+      <c r="AR23" t="s">
+        <v>44</v>
+      </c>
+      <c r="AS23" t="s">
+        <v>44</v>
+      </c>
+      <c r="AT23" t="s">
+        <v>161</v>
+      </c>
+      <c r="AU23" t="s">
+        <v>44</v>
+      </c>
+      <c r="AV23" t="s">
+        <v>44</v>
+      </c>
+      <c r="AW23" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="24" spans="1:49" x14ac:dyDescent="0.45">
+      <c r="A24" t="s">
+        <v>138</v>
+      </c>
+      <c r="V24" t="s">
+        <v>44</v>
+      </c>
+      <c r="W24" t="s">
+        <v>44</v>
+      </c>
+      <c r="X24" t="s">
+        <v>44</v>
+      </c>
+      <c r="Y24" t="s">
+        <v>44</v>
+      </c>
+      <c r="Z24" t="s">
+        <v>161</v>
+      </c>
+      <c r="AA24" t="s">
+        <v>44</v>
+      </c>
+      <c r="AB24" t="s">
+        <v>44</v>
+      </c>
+      <c r="AC24" t="s">
+        <v>44</v>
+      </c>
+      <c r="AD24" t="s">
+        <v>161</v>
+      </c>
+      <c r="AE24" t="s">
+        <v>44</v>
+      </c>
+      <c r="AF24" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="25" spans="1:49" x14ac:dyDescent="0.45">
+      <c r="A25" t="s">
+        <v>164</v>
+      </c>
+      <c r="Z25" t="s">
+        <v>44</v>
+      </c>
+      <c r="AA25" t="s">
+        <v>161</v>
+      </c>
+      <c r="AB25" t="s">
+        <v>161</v>
+      </c>
+      <c r="AC25" t="s">
+        <v>44</v>
+      </c>
+      <c r="AD25" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="26" spans="1:49" x14ac:dyDescent="0.45">
+      <c r="A26" t="s">
+        <v>152</v>
+      </c>
+      <c r="AB26" t="s">
+        <v>44</v>
+      </c>
+      <c r="AC26" t="s">
+        <v>44</v>
+      </c>
+      <c r="AD26" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="27" spans="1:49" x14ac:dyDescent="0.45">
+      <c r="A27" t="s">
+        <v>129</v>
+      </c>
+      <c r="AB27" t="s">
+        <v>44</v>
+      </c>
+      <c r="AC27" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="28" spans="1:49" x14ac:dyDescent="0.45">
+      <c r="A28" t="s">
+        <v>139</v>
+      </c>
+      <c r="G28" t="s">
+        <v>161</v>
+      </c>
+      <c r="H28" t="s">
+        <v>161</v>
+      </c>
+      <c r="I28" t="s">
+        <v>44</v>
+      </c>
+      <c r="J28" t="s">
+        <v>44</v>
+      </c>
+      <c r="K28" t="s">
+        <v>44</v>
+      </c>
+      <c r="L28" t="s">
+        <v>161</v>
+      </c>
+      <c r="M28" t="s">
+        <v>161</v>
+      </c>
+      <c r="N28" t="s">
+        <v>161</v>
+      </c>
+      <c r="O28" t="s">
+        <v>44</v>
+      </c>
+      <c r="P28" t="s">
+        <v>44</v>
+      </c>
+      <c r="Q28" t="s">
+        <v>44</v>
+      </c>
+      <c r="R28" t="s">
+        <v>44</v>
+      </c>
+      <c r="S28" t="s">
+        <v>44</v>
+      </c>
+      <c r="T28" t="s">
+        <v>161</v>
+      </c>
+      <c r="U28" t="s">
+        <v>44</v>
+      </c>
+      <c r="V28" t="s">
+        <v>44</v>
+      </c>
+      <c r="Y28" t="s">
+        <v>44</v>
+      </c>
+      <c r="Z28" t="s">
+        <v>44</v>
+      </c>
+      <c r="AA28" t="s">
+        <v>44</v>
+      </c>
+      <c r="AB28" t="s">
+        <v>44</v>
+      </c>
+      <c r="AC28" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="29" spans="1:49" x14ac:dyDescent="0.45">
+      <c r="A29" t="s">
+        <v>140</v>
+      </c>
+      <c r="N29" t="s">
+        <v>161</v>
+      </c>
+      <c r="O29" t="s">
+        <v>161</v>
+      </c>
+      <c r="P29" t="s">
+        <v>161</v>
+      </c>
+      <c r="Q29" t="s">
+        <v>44</v>
+      </c>
+      <c r="R29" t="s">
+        <v>161</v>
+      </c>
+      <c r="S29" t="s">
+        <v>161</v>
+      </c>
+      <c r="T29" t="s">
+        <v>161</v>
+      </c>
+      <c r="U29" t="s">
+        <v>161</v>
+      </c>
+      <c r="V29" t="s">
+        <v>44</v>
+      </c>
+      <c r="W29" t="s">
+        <v>161</v>
+      </c>
+      <c r="X29" t="s">
+        <v>161</v>
+      </c>
+      <c r="Y29" t="s">
+        <v>44</v>
+      </c>
+      <c r="Z29" t="s">
+        <v>161</v>
+      </c>
+      <c r="AA29" t="s">
+        <v>161</v>
+      </c>
+      <c r="AB29" t="s">
+        <v>161</v>
+      </c>
+      <c r="AC29" t="s">
+        <v>44</v>
+      </c>
+      <c r="AD29" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="30" spans="1:49" x14ac:dyDescent="0.45">
+      <c r="A30" t="s">
+        <v>141</v>
+      </c>
+      <c r="G30" t="s">
+        <v>161</v>
+      </c>
+      <c r="H30" t="s">
+        <v>44</v>
+      </c>
+      <c r="I30" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="31" spans="1:49" x14ac:dyDescent="0.45">
+      <c r="A31" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="32" spans="1:49" x14ac:dyDescent="0.45">
+      <c r="A32" t="s">
+        <v>130</v>
+      </c>
+      <c r="AA32" t="s">
+        <v>44</v>
+      </c>
+      <c r="AB32" t="s">
+        <v>44</v>
+      </c>
+      <c r="AC32" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="33" spans="1:49" x14ac:dyDescent="0.45">
+      <c r="A33" t="s">
+        <v>132</v>
+      </c>
+      <c r="AB33" t="s">
+        <v>44</v>
+      </c>
+      <c r="AC33" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="34" spans="1:49" x14ac:dyDescent="0.45">
+      <c r="A34" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="35" spans="1:49" x14ac:dyDescent="0.45">
+      <c r="A35" t="s">
+        <v>142</v>
+      </c>
+      <c r="G35" t="s">
+        <v>44</v>
+      </c>
+      <c r="H35" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="36" spans="1:49" x14ac:dyDescent="0.45">
+      <c r="A36" t="s">
+        <v>148</v>
+      </c>
+      <c r="O36" t="s">
+        <v>44</v>
+      </c>
+      <c r="P36" t="s">
+        <v>161</v>
+      </c>
+      <c r="Q36" t="s">
+        <v>161</v>
+      </c>
+      <c r="R36" t="s">
+        <v>161</v>
+      </c>
+      <c r="S36" t="s">
+        <v>44</v>
+      </c>
+      <c r="AA36" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="37" spans="1:49" x14ac:dyDescent="0.45">
+      <c r="A37" t="s">
+        <v>149</v>
+      </c>
+      <c r="AA37" t="s">
+        <v>44</v>
+      </c>
+      <c r="AB37" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="39" spans="1:49" x14ac:dyDescent="0.45">
+      <c r="A39" s="1" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="40" spans="1:49" x14ac:dyDescent="0.45">
+      <c r="A40" s="7">
+        <v>1600</v>
+      </c>
+      <c r="U40" t="s">
+        <v>44</v>
+      </c>
+      <c r="V40" t="s">
+        <v>161</v>
+      </c>
+      <c r="W40" t="s">
+        <v>161</v>
+      </c>
+      <c r="X40" t="s">
+        <v>44</v>
+      </c>
+      <c r="Y40" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="41" spans="1:49" x14ac:dyDescent="0.45">
+      <c r="A41" t="s">
+        <v>127</v>
+      </c>
+      <c r="U41" t="s">
+        <v>44</v>
+      </c>
+      <c r="V41" t="s">
+        <v>161</v>
+      </c>
+      <c r="W41" t="s">
+        <v>161</v>
+      </c>
+      <c r="X41" t="s">
+        <v>44</v>
+      </c>
+      <c r="Y41" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="42" spans="1:49" x14ac:dyDescent="0.45">
+      <c r="A42" t="s">
+        <v>125</v>
+      </c>
+      <c r="X42" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="44" spans="1:49" x14ac:dyDescent="0.45">
+      <c r="A44" s="1" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="45" spans="1:49" x14ac:dyDescent="0.45">
+      <c r="A45" t="s">
+        <v>100</v>
+      </c>
+      <c r="M45" t="s">
+        <v>44</v>
+      </c>
+      <c r="N45" t="s">
+        <v>161</v>
+      </c>
+      <c r="O45" t="s">
+        <v>44</v>
+      </c>
+      <c r="P45" t="s">
+        <v>161</v>
+      </c>
+      <c r="Q45" t="s">
+        <v>161</v>
+      </c>
+      <c r="R45" t="s">
+        <v>161</v>
+      </c>
+      <c r="S45" t="s">
+        <v>161</v>
+      </c>
+      <c r="T45" t="s">
+        <v>44</v>
+      </c>
+      <c r="U45" t="s">
+        <v>161</v>
+      </c>
+      <c r="V45" t="s">
+        <v>161</v>
+      </c>
+      <c r="W45" t="s">
+        <v>161</v>
+      </c>
+      <c r="X45" t="s">
+        <v>161</v>
+      </c>
+      <c r="Y45" t="s">
+        <v>161</v>
+      </c>
+      <c r="Z45" t="s">
+        <v>161</v>
+      </c>
+      <c r="AA45" t="s">
+        <v>161</v>
+      </c>
+      <c r="AB45" t="s">
+        <v>161</v>
+      </c>
+      <c r="AC45" t="s">
+        <v>44</v>
+      </c>
+      <c r="AD45" t="s">
+        <v>161</v>
+      </c>
+      <c r="AE45" t="s">
+        <v>161</v>
+      </c>
+      <c r="AF45" t="s">
+        <v>44</v>
+      </c>
+      <c r="AG45" t="s">
+        <v>44</v>
+      </c>
+      <c r="AH45" t="s">
+        <v>44</v>
+      </c>
+      <c r="AI45" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="46" spans="1:49" x14ac:dyDescent="0.45">
+      <c r="A46" t="s">
+        <v>155</v>
+      </c>
+      <c r="AI46" t="s">
+        <v>44</v>
+      </c>
+      <c r="AJ46" t="s">
+        <v>44</v>
+      </c>
+      <c r="AK46" t="s">
+        <v>161</v>
+      </c>
+      <c r="AL46" t="s">
+        <v>161</v>
+      </c>
+      <c r="AM46" t="s">
+        <v>44</v>
+      </c>
+      <c r="AN46" t="s">
+        <v>44</v>
+      </c>
+      <c r="AO46" t="s">
+        <v>44</v>
+      </c>
+      <c r="AP46" t="s">
+        <v>44</v>
+      </c>
+      <c r="AQ46" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="47" spans="1:49" x14ac:dyDescent="0.45">
+      <c r="A47" t="s">
+        <v>156</v>
+      </c>
+      <c r="AI47" t="s">
+        <v>44</v>
+      </c>
+      <c r="AQ47" t="s">
+        <v>44</v>
+      </c>
+      <c r="AR47" t="s">
+        <v>44</v>
+      </c>
+      <c r="AS47" t="s">
+        <v>161</v>
+      </c>
+      <c r="AT47" t="s">
+        <v>44</v>
+      </c>
+      <c r="AU47" t="s">
+        <v>161</v>
+      </c>
+      <c r="AV47" t="s">
+        <v>44</v>
+      </c>
+      <c r="AW47" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="48" spans="1:49" x14ac:dyDescent="0.45">
+      <c r="A48" t="s">
+        <v>126</v>
+      </c>
+      <c r="M48" t="s">
+        <v>44</v>
+      </c>
+      <c r="N48" t="s">
+        <v>161</v>
+      </c>
+      <c r="O48" t="s">
+        <v>44</v>
+      </c>
+      <c r="P48" t="s">
+        <v>161</v>
+      </c>
+      <c r="Q48" t="s">
+        <v>161</v>
+      </c>
+      <c r="R48" t="s">
+        <v>161</v>
+      </c>
+      <c r="S48" t="s">
+        <v>161</v>
+      </c>
+      <c r="T48" t="s">
+        <v>44</v>
+      </c>
+      <c r="U48" t="s">
+        <v>161</v>
+      </c>
+      <c r="V48" t="s">
+        <v>161</v>
+      </c>
+      <c r="W48" t="s">
+        <v>161</v>
+      </c>
+      <c r="X48" t="s">
+        <v>161</v>
+      </c>
+      <c r="Y48" t="s">
+        <v>161</v>
+      </c>
+      <c r="Z48" t="s">
+        <v>161</v>
+      </c>
+      <c r="AA48" t="s">
+        <v>161</v>
+      </c>
+      <c r="AB48" t="s">
+        <v>161</v>
+      </c>
+      <c r="AC48" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="49" spans="1:49" x14ac:dyDescent="0.45">
+      <c r="A49" t="s">
+        <v>137</v>
+      </c>
+      <c r="M49" t="s">
+        <v>44</v>
+      </c>
+      <c r="N49" t="s">
+        <v>161</v>
+      </c>
+      <c r="O49" t="s">
+        <v>161</v>
+      </c>
+      <c r="P49" t="s">
+        <v>161</v>
+      </c>
+      <c r="Q49" t="s">
+        <v>161</v>
+      </c>
+      <c r="R49" t="s">
+        <v>161</v>
+      </c>
+      <c r="S49" t="s">
+        <v>161</v>
+      </c>
+      <c r="T49" t="s">
+        <v>44</v>
+      </c>
+      <c r="U49" t="s">
+        <v>161</v>
+      </c>
+      <c r="V49" t="s">
+        <v>161</v>
+      </c>
+      <c r="W49" t="s">
+        <v>161</v>
+      </c>
+      <c r="X49" t="s">
+        <v>161</v>
+      </c>
+      <c r="Y49" t="s">
+        <v>161</v>
+      </c>
+      <c r="Z49" t="s">
+        <v>161</v>
+      </c>
+      <c r="AA49" t="s">
+        <v>161</v>
+      </c>
+      <c r="AB49" t="s">
+        <v>161</v>
+      </c>
+      <c r="AC49" t="s">
+        <v>161</v>
+      </c>
+      <c r="AD49" t="s">
+        <v>161</v>
+      </c>
+      <c r="AE49" t="s">
+        <v>161</v>
+      </c>
+      <c r="AF49" t="s">
+        <v>44</v>
+      </c>
+      <c r="AG49" t="s">
+        <v>44</v>
+      </c>
+      <c r="AH49" t="s">
+        <v>44</v>
+      </c>
+      <c r="AI49" t="s">
+        <v>44</v>
+      </c>
+      <c r="AJ49" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="50" spans="1:49" x14ac:dyDescent="0.45">
+      <c r="A50" t="s">
+        <v>125</v>
+      </c>
+      <c r="O50" t="s">
+        <v>44</v>
+      </c>
+      <c r="AC50" t="s">
+        <v>44</v>
+      </c>
+      <c r="AD50" t="s">
+        <v>161</v>
+      </c>
+      <c r="AE50" t="s">
+        <v>161</v>
+      </c>
+      <c r="AF50" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="51" spans="1:49" x14ac:dyDescent="0.45">
+      <c r="A51" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="52" spans="1:49" x14ac:dyDescent="0.45">
+      <c r="A52" t="s">
+        <v>136</v>
+      </c>
+      <c r="AF52" t="s">
+        <v>44</v>
+      </c>
+      <c r="AG52" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="53" spans="1:49" x14ac:dyDescent="0.45">
+      <c r="A53" t="s">
+        <v>134</v>
+      </c>
+      <c r="AF53" t="s">
+        <v>44</v>
+      </c>
+      <c r="AG53" t="s">
+        <v>44</v>
+      </c>
+      <c r="AH53" t="s">
+        <v>161</v>
+      </c>
+      <c r="AI53" t="s">
+        <v>44</v>
+      </c>
+      <c r="AJ53" t="s">
+        <v>161</v>
+      </c>
+      <c r="AK53" t="s">
+        <v>161</v>
+      </c>
+      <c r="AL53" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="54" spans="1:49" x14ac:dyDescent="0.45">
+      <c r="A54" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="55" spans="1:49" x14ac:dyDescent="0.45">
+      <c r="A55" t="s">
+        <v>153</v>
+      </c>
+      <c r="AG55" t="s">
+        <v>44</v>
+      </c>
+      <c r="AH55" t="s">
+        <v>44</v>
+      </c>
+      <c r="AL55" t="s">
+        <v>44</v>
+      </c>
+      <c r="AM55" t="s">
+        <v>44</v>
+      </c>
+      <c r="AN55" t="s">
+        <v>161</v>
+      </c>
+      <c r="AO55" t="s">
+        <v>44</v>
+      </c>
+      <c r="AP55" t="s">
+        <v>44</v>
+      </c>
+      <c r="AQ55" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="56" spans="1:49" x14ac:dyDescent="0.45">
+      <c r="A56" t="s">
+        <v>154</v>
+      </c>
+      <c r="AI56" t="s">
+        <v>44</v>
+      </c>
+      <c r="AJ56" t="s">
+        <v>44</v>
+      </c>
+      <c r="AK56" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="57" spans="1:49" x14ac:dyDescent="0.45">
+      <c r="A57" t="s">
+        <v>158</v>
+      </c>
+      <c r="AM57" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="58" spans="1:49" x14ac:dyDescent="0.45">
+      <c r="A58" t="s">
+        <v>159</v>
+      </c>
+      <c r="AI58" t="s">
+        <v>44</v>
+      </c>
+      <c r="AJ58" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="59" spans="1:49" x14ac:dyDescent="0.45">
+      <c r="A59" t="s">
+        <v>22</v>
+      </c>
+      <c r="AN59" t="s">
+        <v>44</v>
+      </c>
+      <c r="AO59" t="s">
+        <v>44</v>
+      </c>
+      <c r="AP59" t="s">
+        <v>44</v>
+      </c>
+      <c r="AQ59" t="s">
+        <v>44</v>
+      </c>
+      <c r="AR59" t="s">
+        <v>44</v>
+      </c>
+      <c r="AS59" t="s">
+        <v>161</v>
+      </c>
+      <c r="AT59" t="s">
+        <v>44</v>
+      </c>
+      <c r="AU59" t="s">
+        <v>161</v>
+      </c>
+      <c r="AV59" t="s">
+        <v>44</v>
+      </c>
+      <c r="AW59" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="61" spans="1:49" x14ac:dyDescent="0.45">
+      <c r="A61" s="1" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="62" spans="1:49" x14ac:dyDescent="0.45">
+      <c r="A62" t="s">
+        <v>155</v>
+      </c>
+      <c r="AK62" t="s">
+        <v>44</v>
+      </c>
+      <c r="AL62" t="s">
+        <v>161</v>
+      </c>
+      <c r="AM62" t="s">
+        <v>44</v>
+      </c>
+      <c r="AN62" t="s">
+        <v>44</v>
+      </c>
+      <c r="AO62" t="s">
+        <v>44</v>
+      </c>
+      <c r="AP62" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="63" spans="1:49" x14ac:dyDescent="0.45">
+      <c r="A63" t="s">
+        <v>156</v>
+      </c>
+      <c r="AI63" t="s">
+        <v>44</v>
+      </c>
+      <c r="AQ63" t="s">
+        <v>44</v>
+      </c>
+      <c r="AR63" t="s">
+        <v>44</v>
+      </c>
+      <c r="AS63" t="s">
+        <v>44</v>
+      </c>
+      <c r="AT63" t="s">
+        <v>44</v>
+      </c>
+      <c r="AU63" t="s">
+        <v>161</v>
+      </c>
+      <c r="AV63" t="s">
+        <v>44</v>
+      </c>
+      <c r="AW63" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="64" spans="1:49" x14ac:dyDescent="0.45">
+      <c r="A64" t="s">
+        <v>160</v>
+      </c>
+      <c r="AN64" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="65" spans="1:49" x14ac:dyDescent="0.45">
+      <c r="A65" t="s">
+        <v>153</v>
+      </c>
+      <c r="AN65" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="66" spans="1:49" x14ac:dyDescent="0.45">
+      <c r="A66" t="s">
+        <v>154</v>
+      </c>
+      <c r="AI66" t="s">
+        <v>44</v>
+      </c>
+      <c r="AN66" t="s">
+        <v>44</v>
+      </c>
+      <c r="AO66" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="67" spans="1:49" x14ac:dyDescent="0.45">
+      <c r="A67" t="s">
+        <v>158</v>
+      </c>
+      <c r="AI67" t="s">
+        <v>44</v>
+      </c>
+      <c r="AJ67" t="s">
+        <v>161</v>
+      </c>
+      <c r="AK67" t="s">
+        <v>44</v>
+      </c>
+      <c r="AL67" t="s">
+        <v>161</v>
+      </c>
+      <c r="AM67" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="68" spans="1:49" x14ac:dyDescent="0.45">
+      <c r="A68" t="s">
+        <v>22</v>
+      </c>
+      <c r="AP68" t="s">
+        <v>44</v>
+      </c>
+      <c r="AQ68" t="s">
+        <v>44</v>
+      </c>
+      <c r="AR68" t="s">
+        <v>44</v>
+      </c>
+      <c r="AS68" t="s">
+        <v>44</v>
+      </c>
+      <c r="AT68" t="s">
+        <v>44</v>
+      </c>
+      <c r="AU68" t="s">
+        <v>161</v>
+      </c>
+      <c r="AV68" t="s">
+        <v>44</v>
+      </c>
+      <c r="AW68" t="s">
+        <v>161</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <legacyDrawing r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{34F6A220-FD91-4F5A-ACFA-A0D4B83AD909}">
   <dimension ref="A1:D13"/>
   <sheetViews>
@@ -2721,7 +4857,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C42AD58B-783D-4A65-88F6-4F4D48B1C5CA}">
   <dimension ref="A1:K32"/>
   <sheetViews>

</xml_diff>